<commit_message>
refactoring and working with the order form output
</commit_message>
<xml_diff>
--- a/calc/static/calc/Piql_order_form.xlsx
+++ b/calc/static/calc/Piql_order_form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="order" sheetId="1" state="visible" r:id="rId1"/>
@@ -312,7 +312,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
@@ -359,75 +359,59 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -436,22 +420,39 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -798,177 +799,178 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="96" zoomScaleNormal="55" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:H4"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScale="96" zoomScaleNormal="55" zoomScalePageLayoutView="96" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="16.5"/>
   <cols>
-    <col width="5.7265625" customWidth="1" style="21" min="1" max="1"/>
-    <col width="9.1796875" customWidth="1" style="21" min="2" max="2"/>
-    <col width="20.08984375" customWidth="1" style="21" min="3" max="3"/>
-    <col width="10.26953125" customWidth="1" style="21" min="4" max="4"/>
-    <col width="9.1796875" customWidth="1" style="21" min="5" max="5"/>
-    <col width="7.54296875" bestFit="1" customWidth="1" style="21" min="6" max="6"/>
-    <col width="11.54296875" bestFit="1" customWidth="1" style="21" min="7" max="7"/>
-    <col width="14" customWidth="1" style="21" min="8" max="8"/>
-    <col width="9.1796875" customWidth="1" style="21" min="9" max="32"/>
-    <col width="9.1796875" customWidth="1" style="21" min="33" max="16384"/>
+    <col width="5.7265625" customWidth="1" style="22" min="1" max="1"/>
+    <col width="9.1796875" customWidth="1" style="22" min="2" max="2"/>
+    <col width="20.08984375" customWidth="1" style="22" min="3" max="3"/>
+    <col width="11.26953125" customWidth="1" style="22" min="4" max="4"/>
+    <col width="9.1796875" customWidth="1" style="22" min="5" max="5"/>
+    <col width="7.54296875" bestFit="1" customWidth="1" style="22" min="6" max="6"/>
+    <col width="11.54296875" bestFit="1" customWidth="1" style="22" min="7" max="7"/>
+    <col width="14" customWidth="1" style="22" min="8" max="8"/>
+    <col width="10.453125" customWidth="1" style="22" min="9" max="9"/>
+    <col width="9.1796875" customWidth="1" style="22" min="10" max="41"/>
+    <col width="9.1796875" customWidth="1" style="22" min="42" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
-      <c r="A1" s="22" t="n"/>
-      <c r="E1" s="55" t="inlineStr">
+      <c r="A1" s="26" t="n"/>
+      <c r="E1" s="21" t="inlineStr">
         <is>
           <t>Partner Order Form</t>
         </is>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
-      <c r="A2" s="22" t="n"/>
+      <c r="A2" s="26" t="n"/>
     </row>
     <row r="3" ht="14.15" customHeight="1">
-      <c r="A3" s="47" t="n"/>
+      <c r="A3" s="41" t="n"/>
     </row>
     <row r="4" ht="14.15" customHeight="1">
-      <c r="A4" s="22" t="n"/>
-      <c r="E4" s="56" t="inlineStr">
+      <c r="A4" s="26" t="n"/>
+      <c r="E4" s="23" t="inlineStr">
         <is>
           <t>Date:</t>
         </is>
       </c>
-      <c r="G4" s="58" t="n">
-        <v>44074.8820765559</v>
+      <c r="G4" s="25" t="n">
+        <v>44075.88390811362</v>
       </c>
     </row>
     <row r="5" ht="14.15" customHeight="1">
-      <c r="A5" s="22" t="n"/>
-      <c r="E5" s="56" t="inlineStr">
+      <c r="A5" s="26" t="n"/>
+      <c r="E5" s="23" t="inlineStr">
         <is>
           <t>Piql Partner:</t>
         </is>
       </c>
-      <c r="G5" s="22" t="n"/>
+      <c r="G5" s="26" t="n"/>
     </row>
     <row r="6" ht="14.15" customHeight="1">
-      <c r="A6" s="22" t="n"/>
-      <c r="E6" s="56" t="inlineStr">
+      <c r="A6" s="26" t="n"/>
+      <c r="E6" s="23" t="inlineStr">
         <is>
           <t>Partner Order Number:</t>
         </is>
       </c>
-      <c r="G6" s="59" t="n"/>
+      <c r="G6" s="27" t="n"/>
     </row>
     <row r="7" ht="14.15" customHeight="1">
-      <c r="A7" s="22" t="n"/>
-      <c r="E7" s="57" t="inlineStr">
+      <c r="A7" s="26" t="n"/>
+      <c r="E7" s="24" t="inlineStr">
         <is>
           <t>Customer name:</t>
         </is>
       </c>
-      <c r="G7" s="22" t="inlineStr">
-        <is>
-          <t>El caracoli</t>
+      <c r="G7" s="26" t="inlineStr">
+        <is>
+          <t>Tamarindo</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="22" t="n"/>
+      <c r="A8" s="26" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="43" t="inlineStr">
+      <c r="A9" s="28" t="inlineStr">
         <is>
           <t>PIQL PARTNER &lt;Mandatory&gt;</t>
         </is>
       </c>
-      <c r="B9" s="24" t="n"/>
-      <c r="C9" s="24" t="n"/>
-      <c r="D9" s="24" t="n"/>
-      <c r="E9" s="33" t="n"/>
-      <c r="F9" s="43" t="inlineStr">
+      <c r="B9" s="29" t="n"/>
+      <c r="C9" s="29" t="n"/>
+      <c r="D9" s="29" t="n"/>
+      <c r="E9" s="30" t="n"/>
+      <c r="F9" s="28" t="inlineStr">
         <is>
           <t>Comments:</t>
         </is>
       </c>
-      <c r="G9" s="24" t="n"/>
-      <c r="H9" s="33" t="n"/>
+      <c r="G9" s="29" t="n"/>
+      <c r="H9" s="30" t="n"/>
     </row>
     <row r="10" ht="17.25" customHeight="1">
-      <c r="A10" s="52" t="inlineStr">
+      <c r="A10" s="46" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="B10" s="40" t="n"/>
-      <c r="C10" s="40" t="n"/>
-      <c r="D10" s="40" t="n"/>
-      <c r="E10" s="41" t="n"/>
-      <c r="F10" s="44" t="inlineStr">
-        <is>
-          <t>ensayando un apropuesta hibrida y el piqlConnect</t>
-        </is>
-      </c>
-      <c r="H10" s="27" t="n"/>
+      <c r="B10" s="47" t="n"/>
+      <c r="C10" s="47" t="n"/>
+      <c r="D10" s="47" t="n"/>
+      <c r="E10" s="48" t="n"/>
+      <c r="F10" s="36" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
+      </c>
+      <c r="H10" s="34" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="26" t="inlineStr">
+      <c r="A11" s="33" t="inlineStr">
         <is>
           <t>Contact person</t>
         </is>
       </c>
-      <c r="E11" s="27" t="n"/>
-      <c r="F11" s="45" t="n"/>
-      <c r="H11" s="27" t="n"/>
+      <c r="E11" s="34" t="n"/>
+      <c r="F11" s="37" t="n"/>
+      <c r="H11" s="34" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="28" t="inlineStr">
+      <c r="A12" s="58" t="inlineStr">
         <is>
           <t>Telephone</t>
         </is>
       </c>
-      <c r="E12" s="27" t="n"/>
-      <c r="F12" s="45" t="n"/>
-      <c r="H12" s="27" t="n"/>
+      <c r="E12" s="34" t="n"/>
+      <c r="F12" s="37" t="n"/>
+      <c r="H12" s="34" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="28" t="inlineStr">
+      <c r="A13" s="58" t="inlineStr">
         <is>
           <t>email:</t>
         </is>
       </c>
-      <c r="E13" s="27" t="n"/>
-      <c r="F13" s="45" t="n"/>
-      <c r="H13" s="27" t="n"/>
+      <c r="E13" s="34" t="n"/>
+      <c r="F13" s="37" t="n"/>
+      <c r="H13" s="34" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="26" t="n"/>
-      <c r="E14" s="27" t="n"/>
-      <c r="F14" s="45" t="n"/>
-      <c r="H14" s="27" t="n"/>
+      <c r="A14" s="33" t="n"/>
+      <c r="E14" s="34" t="n"/>
+      <c r="F14" s="37" t="n"/>
+      <c r="H14" s="34" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="29" t="n"/>
-      <c r="B15" s="30" t="n"/>
-      <c r="C15" s="30" t="n"/>
-      <c r="D15" s="30" t="n"/>
-      <c r="E15" s="31" t="n"/>
-      <c r="F15" s="46" t="n"/>
-      <c r="G15" s="30" t="n"/>
-      <c r="H15" s="31" t="n"/>
+      <c r="A15" s="59" t="n"/>
+      <c r="B15" s="39" t="n"/>
+      <c r="C15" s="39" t="n"/>
+      <c r="D15" s="39" t="n"/>
+      <c r="E15" s="40" t="n"/>
+      <c r="F15" s="38" t="n"/>
+      <c r="G15" s="39" t="n"/>
+      <c r="H15" s="40" t="n"/>
     </row>
     <row r="16" ht="30" customHeight="1">
-      <c r="A16" s="32" t="inlineStr">
+      <c r="A16" s="60" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="B16" s="24" t="n"/>
-      <c r="C16" s="24" t="n"/>
-      <c r="D16" s="24" t="n"/>
-      <c r="E16" s="33" t="n"/>
-      <c r="F16" s="32" t="inlineStr">
+      <c r="B16" s="29" t="n"/>
+      <c r="C16" s="29" t="n"/>
+      <c r="D16" s="29" t="n"/>
+      <c r="E16" s="30" t="n"/>
+      <c r="F16" s="60" t="inlineStr">
         <is>
           <t>Qty</t>
         </is>
@@ -985,45 +987,45 @@
       </c>
     </row>
     <row r="17" ht="17.25" customHeight="1">
-      <c r="A17" s="34" t="inlineStr">
+      <c r="A17" s="35" t="inlineStr">
         <is>
           <t xml:space="preserve">1. Offline Storage </t>
         </is>
       </c>
-      <c r="B17" s="24" t="n"/>
-      <c r="C17" s="24" t="n"/>
-      <c r="D17" s="24" t="n"/>
-      <c r="E17" s="33" t="n"/>
+      <c r="B17" s="29" t="n"/>
+      <c r="C17" s="29" t="n"/>
+      <c r="D17" s="29" t="n"/>
+      <c r="E17" s="30" t="n"/>
       <c r="F17" s="2" t="n"/>
       <c r="G17" s="9" t="n"/>
       <c r="H17" s="10" t="n"/>
     </row>
     <row r="18" ht="16.5" customHeight="1">
-      <c r="A18" s="35" t="inlineStr">
+      <c r="A18" s="32" t="inlineStr">
         <is>
           <t>piqlConnect (only piqlFilm)</t>
         </is>
       </c>
-      <c r="B18" s="24" t="n"/>
-      <c r="C18" s="24" t="n"/>
-      <c r="D18" s="24" t="n"/>
-      <c r="E18" s="33" t="n"/>
+      <c r="B18" s="29" t="n"/>
+      <c r="C18" s="29" t="n"/>
+      <c r="D18" s="29" t="n"/>
+      <c r="E18" s="30" t="n"/>
       <c r="F18" s="2" t="n"/>
       <c r="G18" s="9" t="n"/>
       <c r="H18" s="10" t="n"/>
     </row>
     <row r="19" ht="17.25" customHeight="1">
-      <c r="A19" s="35" t="inlineStr">
+      <c r="A19" s="32" t="inlineStr">
         <is>
           <t>Digital (GB)</t>
         </is>
       </c>
-      <c r="B19" s="24" t="n"/>
-      <c r="C19" s="24" t="n"/>
-      <c r="D19" s="24" t="n"/>
-      <c r="E19" s="33" t="n"/>
+      <c r="B19" s="29" t="n"/>
+      <c r="C19" s="29" t="n"/>
+      <c r="D19" s="29" t="n"/>
+      <c r="E19" s="30" t="n"/>
       <c r="F19" s="14" t="n">
-        <v>240</v>
+        <v>120</v>
       </c>
       <c r="G19" s="9" t="n">
         <v>15</v>
@@ -1031,63 +1033,56 @@
       <c r="H19" s="10" t="n">
         <v>1800</v>
       </c>
+      <c r="I19" s="16" t="n"/>
     </row>
     <row r="20" ht="17.25" customHeight="1">
-      <c r="A20" s="36" t="inlineStr">
+      <c r="A20" s="31" t="inlineStr">
         <is>
           <t>Visual (pages)</t>
         </is>
       </c>
-      <c r="B20" s="24" t="n"/>
-      <c r="C20" s="24" t="n"/>
+      <c r="B20" s="29" t="n"/>
+      <c r="C20" s="29" t="n"/>
       <c r="D20" s="7" t="inlineStr">
         <is>
           <t>Pages/frame:</t>
         </is>
       </c>
-      <c r="E20" s="8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F20" s="15" t="n">
-        <v>650000</v>
-      </c>
-      <c r="G20" s="11" t="n">
-        <v>0.016</v>
-      </c>
-      <c r="H20" s="10" t="n">
-        <v>8320</v>
-      </c>
+      <c r="E20" s="8" t="n"/>
+      <c r="F20" s="15" t="n"/>
+      <c r="G20" s="11" t="n"/>
+      <c r="H20" s="10" t="n"/>
+      <c r="I20" s="16" t="n"/>
     </row>
     <row r="21" ht="17.25" customHeight="1">
-      <c r="A21" s="34" t="inlineStr">
+      <c r="A21" s="35" t="inlineStr">
         <is>
           <t>2. Online Storage (GB) - piqlConnect (1TB &amp; 1 piqlFilm included)</t>
         </is>
       </c>
-      <c r="B21" s="24" t="n"/>
-      <c r="C21" s="24" t="n"/>
-      <c r="D21" s="24" t="n"/>
-      <c r="E21" s="33" t="n"/>
+      <c r="B21" s="29" t="n"/>
+      <c r="C21" s="29" t="n"/>
+      <c r="D21" s="29" t="n"/>
+      <c r="E21" s="30" t="n"/>
       <c r="F21" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G21" s="9" t="n">
-        <v>8880</v>
+        <v>0</v>
       </c>
       <c r="H21" s="10" t="n">
-        <v>8880</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I21" s="16" t="n"/>
     </row>
     <row r="22" ht="17.25" customHeight="1">
-      <c r="A22" s="36" t="inlineStr">
+      <c r="A22" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Online Storage (GB) </t>
         </is>
       </c>
-      <c r="B22" s="24" t="n"/>
-      <c r="C22" s="24" t="n"/>
+      <c r="B22" s="29" t="n"/>
+      <c r="C22" s="29" t="n"/>
       <c r="D22" s="3" t="inlineStr">
         <is>
           <t>Payment:</t>
@@ -1095,372 +1090,327 @@
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>yearly</t>
+          <t>only_piqlfilm</t>
         </is>
       </c>
       <c r="F22" s="2" t="n">
-        <v>8000</v>
-      </c>
-      <c r="G22" s="11" t="n">
-        <v>0.576</v>
-      </c>
-      <c r="H22" s="10" t="n">
-        <v>4032</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G22" s="11" t="n"/>
+      <c r="H22" s="10" t="inlineStr">
+        <is>
+          <t>only_piqlfilm</t>
+        </is>
+      </c>
+      <c r="I22" s="16" t="n"/>
     </row>
     <row r="23" ht="17.25" customHeight="1">
-      <c r="A23" s="34" t="inlineStr">
+      <c r="A23" s="35" t="inlineStr">
         <is>
           <t xml:space="preserve">3. Arctic World Archive </t>
         </is>
       </c>
-      <c r="B23" s="24" t="n"/>
-      <c r="C23" s="24" t="n"/>
-      <c r="D23" s="24" t="n"/>
-      <c r="E23" s="33" t="n"/>
+      <c r="B23" s="29" t="n"/>
+      <c r="C23" s="29" t="n"/>
+      <c r="D23" s="29" t="n"/>
+      <c r="E23" s="30" t="n"/>
       <c r="F23" s="2" t="n"/>
       <c r="G23" s="9" t="n"/>
       <c r="H23" s="10" t="n"/>
+      <c r="I23" s="16" t="n"/>
     </row>
     <row r="24" ht="16.5" customHeight="1">
-      <c r="A24" s="35" t="inlineStr">
+      <c r="A24" s="32" t="inlineStr">
         <is>
           <t>Registration fee</t>
         </is>
       </c>
-      <c r="B24" s="24" t="n"/>
-      <c r="C24" s="24" t="n"/>
-      <c r="D24" s="24" t="n"/>
-      <c r="E24" s="33" t="n"/>
-      <c r="F24" s="2" t="n">
+      <c r="B24" s="29" t="n"/>
+      <c r="C24" s="29" t="n"/>
+      <c r="D24" s="29" t="n"/>
+      <c r="E24" s="30" t="n"/>
+      <c r="F24" s="2" t="n"/>
+      <c r="G24" s="9" t="n"/>
+      <c r="H24" s="10" t="n"/>
+      <c r="I24" s="16" t="n"/>
+    </row>
+    <row r="25" ht="16.5" customHeight="1">
+      <c r="A25" s="31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AWA contribution </t>
+        </is>
+      </c>
+      <c r="B25" s="29" t="n"/>
+      <c r="C25" s="29" t="n"/>
+      <c r="D25" s="3" t="inlineStr">
+        <is>
+          <t>Entity:</t>
+        </is>
+      </c>
+      <c r="E25" s="4" t="n"/>
+      <c r="F25" s="2" t="n"/>
+      <c r="G25" s="9" t="n"/>
+      <c r="H25" s="10" t="n"/>
+      <c r="I25" s="16" t="n"/>
+    </row>
+    <row r="26" ht="16.5" customHeight="1">
+      <c r="A26" s="32" t="inlineStr">
+        <is>
+          <t>Management fee (per year)</t>
+        </is>
+      </c>
+      <c r="B26" s="29" t="n"/>
+      <c r="C26" s="29" t="n"/>
+      <c r="D26" s="29" t="n"/>
+      <c r="E26" s="30" t="n"/>
+      <c r="F26" s="2" t="n"/>
+      <c r="G26" s="9" t="n"/>
+      <c r="H26" s="10" t="n"/>
+      <c r="I26" s="16" t="n"/>
+    </row>
+    <row r="27" ht="17.5" customHeight="1">
+      <c r="A27" s="31" t="inlineStr">
+        <is>
+          <t>Storage (reels/ per year)</t>
+        </is>
+      </c>
+      <c r="B27" s="29" t="n"/>
+      <c r="C27" s="29" t="n"/>
+      <c r="D27" s="3" t="inlineStr">
+        <is>
+          <t>Period (years):</t>
+        </is>
+      </c>
+      <c r="E27" s="4" t="n"/>
+      <c r="F27" s="2" t="n"/>
+      <c r="G27" s="9" t="n"/>
+      <c r="H27" s="10" t="n"/>
+      <c r="I27" s="16" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="35" t="inlineStr">
+        <is>
+          <t>4. Professional Services (per day)</t>
+        </is>
+      </c>
+      <c r="B28" s="29" t="n"/>
+      <c r="C28" s="29" t="n"/>
+      <c r="D28" s="29" t="n"/>
+      <c r="E28" s="30" t="n"/>
+      <c r="F28" s="2" t="n"/>
+      <c r="G28" s="9" t="n"/>
+      <c r="H28" s="10" t="n"/>
+      <c r="I28" s="16" t="n"/>
+    </row>
+    <row r="29" ht="15.5" customHeight="1">
+      <c r="A29" s="35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5. piqlReader </t>
+        </is>
+      </c>
+      <c r="B29" s="29" t="n"/>
+      <c r="C29" s="29" t="n"/>
+      <c r="D29" s="29" t="n"/>
+      <c r="E29" s="30" t="n"/>
+      <c r="F29" s="2" t="n"/>
+      <c r="G29" s="9" t="n"/>
+      <c r="H29" s="10" t="n"/>
+      <c r="I29" s="16" t="n"/>
+    </row>
+    <row r="30" ht="17.25" customHeight="1">
+      <c r="A30" s="32" t="inlineStr">
+        <is>
+          <t>Installation and training</t>
+        </is>
+      </c>
+      <c r="B30" s="29" t="n"/>
+      <c r="C30" s="29" t="n"/>
+      <c r="D30" s="29" t="n"/>
+      <c r="E30" s="30" t="n"/>
+      <c r="F30" s="2" t="n"/>
+      <c r="G30" s="9" t="n"/>
+      <c r="H30" s="10" t="n"/>
+      <c r="I30" s="16" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="57" t="inlineStr">
+        <is>
+          <t>Service agreement (per year)</t>
+        </is>
+      </c>
+      <c r="B31" s="29" t="n"/>
+      <c r="C31" s="29" t="n"/>
+      <c r="D31" s="5" t="inlineStr">
+        <is>
+          <t>Type:</t>
+        </is>
+      </c>
+      <c r="E31" s="6" t="n"/>
+      <c r="F31" s="2" t="n"/>
+      <c r="G31" s="9" t="n"/>
+      <c r="H31" s="10" t="n"/>
+      <c r="I31" s="16" t="n"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="56" t="inlineStr">
+        <is>
+          <t>6. Shipment cost</t>
+        </is>
+      </c>
+      <c r="B32" s="29" t="n"/>
+      <c r="C32" s="29" t="n"/>
+      <c r="D32" s="5" t="inlineStr">
+        <is>
+          <t>Reels</t>
+        </is>
+      </c>
+      <c r="E32" s="6" t="n">
         <v>1</v>
-      </c>
-      <c r="G24" s="9" t="n">
-        <v>200</v>
-      </c>
-      <c r="H24" s="10" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="25" ht="16.5" customHeight="1">
-      <c r="A25" s="36" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AWA contribution </t>
-        </is>
-      </c>
-      <c r="B25" s="24" t="n"/>
-      <c r="C25" s="24" t="n"/>
-      <c r="D25" s="3" t="inlineStr">
-        <is>
-          <t>Entity:</t>
-        </is>
-      </c>
-      <c r="E25" s="4" t="inlineStr">
-        <is>
-          <t>public</t>
-        </is>
-      </c>
-      <c r="F25" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G25" s="9" t="n">
-        <v>500</v>
-      </c>
-      <c r="H25" s="10" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="26" ht="16.5" customHeight="1">
-      <c r="A26" s="35" t="inlineStr">
-        <is>
-          <t>Management fee (per year)</t>
-        </is>
-      </c>
-      <c r="B26" s="24" t="n"/>
-      <c r="C26" s="24" t="n"/>
-      <c r="D26" s="24" t="n"/>
-      <c r="E26" s="33" t="n"/>
-      <c r="F26" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G26" s="9" t="n">
-        <v>60</v>
-      </c>
-      <c r="H26" s="10" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" ht="17.5" customHeight="1">
-      <c r="A27" s="36" t="inlineStr">
-        <is>
-          <t>Storage (reels/ per year)</t>
-        </is>
-      </c>
-      <c r="B27" s="24" t="n"/>
-      <c r="C27" s="24" t="n"/>
-      <c r="D27" s="3" t="inlineStr">
-        <is>
-          <t>Period (years):</t>
-        </is>
-      </c>
-      <c r="E27" s="4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="F27" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="G27" s="9" t="n">
-        <v>60</v>
-      </c>
-      <c r="H27" s="10" t="n">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="34" t="inlineStr">
-        <is>
-          <t>4. Professional Services (per day)</t>
-        </is>
-      </c>
-      <c r="B28" s="24" t="n"/>
-      <c r="C28" s="24" t="n"/>
-      <c r="D28" s="24" t="n"/>
-      <c r="E28" s="33" t="n"/>
-      <c r="F28" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="G28" s="9" t="n">
-        <v>900</v>
-      </c>
-      <c r="H28" s="10" t="n">
-        <v>13500</v>
-      </c>
-    </row>
-    <row r="29" ht="15.5" customHeight="1">
-      <c r="A29" s="34" t="inlineStr">
-        <is>
-          <t xml:space="preserve">5. piqlReader </t>
-        </is>
-      </c>
-      <c r="B29" s="24" t="n"/>
-      <c r="C29" s="24" t="n"/>
-      <c r="D29" s="24" t="n"/>
-      <c r="E29" s="33" t="n"/>
-      <c r="F29" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="9" t="n">
-        <v>79900</v>
-      </c>
-      <c r="H29" s="10" t="n">
-        <v>79900</v>
-      </c>
-    </row>
-    <row r="30" ht="17.25" customHeight="1">
-      <c r="A30" s="35" t="inlineStr">
-        <is>
-          <t>Installation and training</t>
-        </is>
-      </c>
-      <c r="B30" s="24" t="n"/>
-      <c r="C30" s="24" t="n"/>
-      <c r="D30" s="24" t="n"/>
-      <c r="E30" s="33" t="n"/>
-      <c r="F30" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="9" t="n">
-        <v>3000</v>
-      </c>
-      <c r="H30" s="10" t="n">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="25" t="inlineStr">
-        <is>
-          <t>Service agreement (per year)</t>
-        </is>
-      </c>
-      <c r="B31" s="24" t="n"/>
-      <c r="C31" s="24" t="n"/>
-      <c r="D31" s="5" t="inlineStr">
-        <is>
-          <t>Type:</t>
-        </is>
-      </c>
-      <c r="E31" s="6" t="inlineStr">
-        <is>
-          <t>gold</t>
-        </is>
-      </c>
-      <c r="F31" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G31" s="9" t="n">
-        <v>2500</v>
-      </c>
-      <c r="H31" s="10" t="n">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="23" t="inlineStr">
-        <is>
-          <t>6. Shipment cost</t>
-        </is>
-      </c>
-      <c r="B32" s="24" t="n"/>
-      <c r="C32" s="24" t="n"/>
-      <c r="D32" s="5" t="inlineStr">
-        <is>
-          <t>Reels</t>
-        </is>
-      </c>
-      <c r="E32" s="6" t="n">
-        <v>7</v>
       </c>
       <c r="F32" s="2" t="n"/>
       <c r="G32" s="9" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H32" s="10" t="n">
-        <v>15892</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="I32" s="16" t="n"/>
     </row>
     <row r="33" ht="16.5" customHeight="1">
-      <c r="A33" s="37" t="n"/>
-      <c r="G33" s="39" t="inlineStr">
+      <c r="A33" s="51" t="n"/>
+      <c r="G33" s="53" t="inlineStr">
         <is>
           <t xml:space="preserve">TOTAL </t>
         </is>
       </c>
       <c r="H33" s="12" t="n">
-        <v>123112</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="42" t="n"/>
-      <c r="D34" s="27" t="n"/>
-      <c r="E34" s="39" t="inlineStr">
+      <c r="A34" s="54" t="n"/>
+      <c r="D34" s="34" t="n"/>
+      <c r="E34" s="53" t="inlineStr">
         <is>
           <t>Total to pay from the second term</t>
         </is>
       </c>
-      <c r="F34" s="40" t="n"/>
-      <c r="G34" s="41" t="n"/>
+      <c r="F34" s="47" t="n"/>
+      <c r="G34" s="48" t="n"/>
       <c r="H34" s="13" t="n">
-        <v>15892</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="22" t="n"/>
+      <c r="A35" s="26" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="38" t="inlineStr">
+      <c r="A36" s="52" t="inlineStr">
         <is>
           <t>Delivery terms: three weeks after the data is received by Piql. ExWorks, Drammen.</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="20" t="inlineStr">
+      <c r="A37" s="55" t="inlineStr">
         <is>
           <t xml:space="preserve">Payment terms 100% on delivery </t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="38" t="inlineStr">
+      <c r="A38" s="52" t="inlineStr">
         <is>
           <t xml:space="preserve">Notes: To provide technical and account information to the production department. Fill out this form: </t>
         </is>
       </c>
-      <c r="B38" s="38" t="n"/>
-      <c r="C38" s="38" t="n"/>
-      <c r="D38" s="38" t="n"/>
-      <c r="E38" s="38" t="n"/>
-      <c r="F38" s="38" t="n"/>
-      <c r="G38" s="38" t="n"/>
-      <c r="H38" s="38" t="n"/>
+      <c r="B38" s="52" t="n"/>
+      <c r="C38" s="52" t="n"/>
+      <c r="D38" s="52" t="n"/>
+      <c r="E38" s="52" t="n"/>
+      <c r="F38" s="52" t="n"/>
+      <c r="G38" s="52" t="n"/>
+      <c r="H38" s="52" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="54" t="inlineStr">
+      <c r="A39" s="50" t="inlineStr">
         <is>
           <t>https://forms.office.com/Pages/ResponsePage.aspx?id=k4yqUSxZRkSwWH0R7QU1A3pm4lZOZiVDhXIaxSEWbBVUM1NPUEw3OTcwMTNLQTcwVzNNOVFST1NEOC4u</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="50" t="n"/>
+      <c r="A40" s="44" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="47" t="inlineStr">
+      <c r="A41" s="41" t="inlineStr">
         <is>
           <t>Send this order to orders@piql.com. If you have any questions concerning this ORDER please contact:</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="51" t="inlineStr">
+      <c r="A42" s="45" t="inlineStr">
         <is>
           <t>Espen Berge Kvam</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="53" t="inlineStr">
+      <c r="A43" s="49" t="inlineStr">
         <is>
           <t>espen.berge.kvam@piql.com</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="48" t="inlineStr">
+      <c r="A44" s="42" t="inlineStr">
         <is>
           <t>+47 94030050</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="47" t="n"/>
+      <c r="A45" s="41" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="47" t="n"/>
+      <c r="A46" s="41" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="21" t="n"/>
+      <c r="A47" s="22" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="49" t="n"/>
+      <c r="A48" s="43" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="21" t="n"/>
+      <c r="A49" s="22" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="E1:H2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="A34:D34"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F10:H15"/>
     <mergeCell ref="A3:H3"/>
@@ -1477,30 +1427,26 @@
     <mergeCell ref="A45:H45"/>
     <mergeCell ref="A46:H46"/>
     <mergeCell ref="A39:H39"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E1:H2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A39" r:id="rId1"/>

</xml_diff>

<commit_message>
adding order.py - populating excel
</commit_message>
<xml_diff>
--- a/calc/static/calc/Piql_order_form.xlsx
+++ b/calc/static/calc/Piql_order_form.xlsx
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="G4" s="25" t="n">
-        <v>44075.88390811362</v>
+        <v>44042.80167855266</v>
       </c>
     </row>
     <row r="5" ht="14.15" customHeight="1">
@@ -872,7 +872,7 @@
       </c>
       <c r="G7" s="26" t="inlineStr">
         <is>
-          <t>Tamarindo</t>
+          <t>Camisas Ramiro</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       <c r="E10" s="48" t="n"/>
       <c r="F10" s="36" t="inlineStr">
         <is>
-          <t>hola</t>
+          <t>qw</t>
         </is>
       </c>
       <c r="H10" s="34" t="n"/>
@@ -1025,7 +1025,7 @@
       <c r="D19" s="29" t="n"/>
       <c r="E19" s="30" t="n"/>
       <c r="F19" s="14" t="n">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="G19" s="9" t="n">
         <v>15</v>
@@ -1068,10 +1068,10 @@
         <v>1</v>
       </c>
       <c r="G21" s="9" t="n">
-        <v>0</v>
+        <v>8880</v>
       </c>
       <c r="H21" s="10" t="n">
-        <v>0</v>
+        <v>8880</v>
       </c>
       <c r="I21" s="16" t="n"/>
     </row>
@@ -1090,17 +1090,17 @@
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
-          <t>only_piqlfilm</t>
+          <t>yearly</t>
         </is>
       </c>
       <c r="F22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="11" t="n"/>
-      <c r="H22" s="10" t="inlineStr">
-        <is>
-          <t>only_piqlfilm</t>
-        </is>
+        <v>2000</v>
+      </c>
+      <c r="G22" s="11" t="n">
+        <v>0.576</v>
+      </c>
+      <c r="H22" s="10" t="n">
+        <v>576</v>
       </c>
       <c r="I22" s="16" t="n"/>
     </row>
@@ -1265,14 +1265,14 @@
         </is>
       </c>
       <c r="E32" s="6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F32" s="2" t="n"/>
       <c r="G32" s="9" t="n">
         <v>30</v>
       </c>
       <c r="H32" s="10" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="I32" s="16" t="n"/>
     </row>
@@ -1284,7 +1284,7 @@
         </is>
       </c>
       <c r="H33" s="12" t="n">
-        <v>3300</v>
+        <v>11256</v>
       </c>
     </row>
     <row r="34">
@@ -1298,7 +1298,7 @@
       <c r="F34" s="47" t="n"/>
       <c r="G34" s="48" t="n"/>
       <c r="H34" s="13" t="n">
-        <v>0</v>
+        <v>9456</v>
       </c>
     </row>
     <row r="35">

</xml_diff>

<commit_message>
users see only the content they created.
</commit_message>
<xml_diff>
--- a/calc/static/calc/Piql_order_form.xlsx
+++ b/calc/static/calc/Piql_order_form.xlsx
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="G4" s="25" t="n">
-        <v>44042.80167855266</v>
+        <v>44076.78246170176</v>
       </c>
     </row>
     <row r="5" ht="14.15" customHeight="1">
@@ -872,7 +872,7 @@
       </c>
       <c r="G7" s="26" t="inlineStr">
         <is>
-          <t>Camisas Ramiro</t>
+          <t>FMU</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       <c r="E10" s="48" t="n"/>
       <c r="F10" s="36" t="inlineStr">
         <is>
-          <t>qw</t>
+          <t>Let's see what is it</t>
         </is>
       </c>
       <c r="H10" s="34" t="n"/>
@@ -1025,13 +1025,13 @@
       <c r="D19" s="29" t="n"/>
       <c r="E19" s="30" t="n"/>
       <c r="F19" s="14" t="n">
-        <v>240</v>
+        <v>3000</v>
       </c>
       <c r="G19" s="9" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" s="10" t="n">
-        <v>1800</v>
+        <v>40320</v>
       </c>
       <c r="I19" s="16" t="n"/>
     </row>
@@ -1094,13 +1094,13 @@
         </is>
       </c>
       <c r="F22" s="2" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="G22" s="11" t="n">
         <v>0.576</v>
       </c>
       <c r="H22" s="10" t="n">
-        <v>576</v>
+        <v>1152</v>
       </c>
       <c r="I22" s="16" t="n"/>
     </row>
@@ -1129,9 +1129,15 @@
       <c r="C24" s="29" t="n"/>
       <c r="D24" s="29" t="n"/>
       <c r="E24" s="30" t="n"/>
-      <c r="F24" s="2" t="n"/>
-      <c r="G24" s="9" t="n"/>
-      <c r="H24" s="10" t="n"/>
+      <c r="F24" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" s="9" t="n">
+        <v>200</v>
+      </c>
+      <c r="H24" s="10" t="n">
+        <v>200</v>
+      </c>
       <c r="I24" s="16" t="n"/>
     </row>
     <row r="25" ht="16.5" customHeight="1">
@@ -1147,10 +1153,20 @@
           <t>Entity:</t>
         </is>
       </c>
-      <c r="E25" s="4" t="n"/>
-      <c r="F25" s="2" t="n"/>
-      <c r="G25" s="9" t="n"/>
-      <c r="H25" s="10" t="n"/>
+      <c r="E25" s="4" t="inlineStr">
+        <is>
+          <t>public</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="9" t="n">
+        <v>500</v>
+      </c>
+      <c r="H25" s="10" t="n">
+        <v>500</v>
+      </c>
       <c r="I25" s="16" t="n"/>
     </row>
     <row r="26" ht="16.5" customHeight="1">
@@ -1163,9 +1179,15 @@
       <c r="C26" s="29" t="n"/>
       <c r="D26" s="29" t="n"/>
       <c r="E26" s="30" t="n"/>
-      <c r="F26" s="2" t="n"/>
-      <c r="G26" s="9" t="n"/>
-      <c r="H26" s="10" t="n"/>
+      <c r="F26" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="9" t="n">
+        <v>60</v>
+      </c>
+      <c r="H26" s="10" t="n">
+        <v>60</v>
+      </c>
       <c r="I26" s="16" t="n"/>
     </row>
     <row r="27" ht="17.5" customHeight="1">
@@ -1181,10 +1203,20 @@
           <t>Period (years):</t>
         </is>
       </c>
-      <c r="E27" s="4" t="n"/>
-      <c r="F27" s="2" t="n"/>
-      <c r="G27" s="9" t="n"/>
-      <c r="H27" s="10" t="n"/>
+      <c r="E27" s="4" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="G27" s="9" t="n">
+        <v>40</v>
+      </c>
+      <c r="H27" s="10" t="n">
+        <v>25000</v>
+      </c>
       <c r="I27" s="16" t="n"/>
     </row>
     <row r="28">
@@ -1212,9 +1244,15 @@
       <c r="C29" s="29" t="n"/>
       <c r="D29" s="29" t="n"/>
       <c r="E29" s="30" t="n"/>
-      <c r="F29" s="2" t="n"/>
-      <c r="G29" s="9" t="n"/>
-      <c r="H29" s="10" t="n"/>
+      <c r="F29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="9" t="n">
+        <v>79900</v>
+      </c>
+      <c r="H29" s="10" t="n">
+        <v>79900</v>
+      </c>
       <c r="I29" s="16" t="n"/>
     </row>
     <row r="30" ht="17.25" customHeight="1">
@@ -1227,9 +1265,15 @@
       <c r="C30" s="29" t="n"/>
       <c r="D30" s="29" t="n"/>
       <c r="E30" s="30" t="n"/>
-      <c r="F30" s="2" t="n"/>
-      <c r="G30" s="9" t="n"/>
-      <c r="H30" s="10" t="n"/>
+      <c r="F30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="9" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H30" s="10" t="n">
+        <v>3000</v>
+      </c>
       <c r="I30" s="16" t="n"/>
     </row>
     <row r="31">
@@ -1245,10 +1289,20 @@
           <t>Type:</t>
         </is>
       </c>
-      <c r="E31" s="6" t="n"/>
-      <c r="F31" s="2" t="n"/>
-      <c r="G31" s="9" t="n"/>
-      <c r="H31" s="10" t="n"/>
+      <c r="E31" s="6" t="inlineStr">
+        <is>
+          <t>gold</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="9" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H31" s="10" t="n">
+        <v>2500</v>
+      </c>
       <c r="I31" s="16" t="n"/>
     </row>
     <row r="32">
@@ -1265,14 +1319,14 @@
         </is>
       </c>
       <c r="E32" s="6" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="F32" s="2" t="n"/>
       <c r="G32" s="9" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H32" s="10" t="n">
-        <v>60</v>
+        <v>500</v>
       </c>
       <c r="I32" s="16" t="n"/>
     </row>
@@ -1284,7 +1338,7 @@
         </is>
       </c>
       <c r="H33" s="12" t="n">
-        <v>11256</v>
+        <v>162952</v>
       </c>
     </row>
     <row r="34">
@@ -1298,7 +1352,7 @@
       <c r="F34" s="47" t="n"/>
       <c r="G34" s="48" t="n"/>
       <c r="H34" s="13" t="n">
-        <v>9456</v>
+        <v>12532</v>
       </c>
     </row>
     <row r="35">

</xml_diff>

<commit_message>
Adding film.py to calculate the piqlFilm price
</commit_message>
<xml_diff>
--- a/calc/static/calc/Piql_order_form.xlsx
+++ b/calc/static/calc/Piql_order_form.xlsx
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="G4" s="25" t="n">
-        <v>44076.78246170176</v>
+        <v>44079.51026330685</v>
       </c>
     </row>
     <row r="5" ht="14.15" customHeight="1">
@@ -872,7 +872,7 @@
       </c>
       <c r="G7" s="26" t="inlineStr">
         <is>
-          <t>FMU</t>
+          <t>Unesco</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       <c r="E10" s="48" t="n"/>
       <c r="F10" s="36" t="inlineStr">
         <is>
-          <t>Let's see what is it</t>
+          <t>test</t>
         </is>
       </c>
       <c r="H10" s="34" t="n"/>
@@ -1010,9 +1010,15 @@
       <c r="C18" s="29" t="n"/>
       <c r="D18" s="29" t="n"/>
       <c r="E18" s="30" t="n"/>
-      <c r="F18" s="2" t="n"/>
-      <c r="G18" s="9" t="n"/>
-      <c r="H18" s="10" t="n"/>
+      <c r="F18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="9" t="n">
+        <v>1500</v>
+      </c>
+      <c r="H18" s="10" t="n">
+        <v>1500</v>
+      </c>
     </row>
     <row r="19" ht="17.25" customHeight="1">
       <c r="A19" s="32" t="inlineStr">
@@ -1024,15 +1030,9 @@
       <c r="C19" s="29" t="n"/>
       <c r="D19" s="29" t="n"/>
       <c r="E19" s="30" t="n"/>
-      <c r="F19" s="14" t="n">
-        <v>3000</v>
-      </c>
-      <c r="G19" s="9" t="n">
-        <v>14</v>
-      </c>
-      <c r="H19" s="10" t="n">
-        <v>40320</v>
-      </c>
+      <c r="F19" s="14" t="n"/>
+      <c r="G19" s="9" t="n"/>
+      <c r="H19" s="10" t="n"/>
       <c r="I19" s="16" t="n"/>
     </row>
     <row r="20" ht="17.25" customHeight="1">
@@ -1048,10 +1048,20 @@
           <t>Pages/frame:</t>
         </is>
       </c>
-      <c r="E20" s="8" t="n"/>
-      <c r="F20" s="15" t="n"/>
-      <c r="G20" s="11" t="n"/>
-      <c r="H20" s="10" t="n"/>
+      <c r="E20" s="8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F20" s="15" t="n">
+        <v>67000</v>
+      </c>
+      <c r="G20" s="11" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="H20" s="10" t="n">
+        <v>2010</v>
+      </c>
       <c r="I20" s="16" t="n"/>
     </row>
     <row r="21" ht="17.25" customHeight="1">
@@ -1064,15 +1074,9 @@
       <c r="C21" s="29" t="n"/>
       <c r="D21" s="29" t="n"/>
       <c r="E21" s="30" t="n"/>
-      <c r="F21" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="9" t="n">
-        <v>8880</v>
-      </c>
-      <c r="H21" s="10" t="n">
-        <v>8880</v>
-      </c>
+      <c r="F21" s="2" t="n"/>
+      <c r="G21" s="9" t="n"/>
+      <c r="H21" s="10" t="n"/>
       <c r="I21" s="16" t="n"/>
     </row>
     <row r="22" ht="17.25" customHeight="1">
@@ -1088,20 +1092,10 @@
           <t>Payment:</t>
         </is>
       </c>
-      <c r="E22" s="4" t="inlineStr">
-        <is>
-          <t>yearly</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="n">
-        <v>3000</v>
-      </c>
-      <c r="G22" s="11" t="n">
-        <v>0.576</v>
-      </c>
-      <c r="H22" s="10" t="n">
-        <v>1152</v>
-      </c>
+      <c r="E22" s="4" t="n"/>
+      <c r="F22" s="2" t="n"/>
+      <c r="G22" s="11" t="n"/>
+      <c r="H22" s="10" t="n"/>
       <c r="I22" s="16" t="n"/>
     </row>
     <row r="23" ht="17.25" customHeight="1">
@@ -1129,15 +1123,9 @@
       <c r="C24" s="29" t="n"/>
       <c r="D24" s="29" t="n"/>
       <c r="E24" s="30" t="n"/>
-      <c r="F24" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G24" s="9" t="n">
-        <v>200</v>
-      </c>
-      <c r="H24" s="10" t="n">
-        <v>200</v>
-      </c>
+      <c r="F24" s="2" t="n"/>
+      <c r="G24" s="9" t="n"/>
+      <c r="H24" s="10" t="n"/>
       <c r="I24" s="16" t="n"/>
     </row>
     <row r="25" ht="16.5" customHeight="1">
@@ -1153,20 +1141,10 @@
           <t>Entity:</t>
         </is>
       </c>
-      <c r="E25" s="4" t="inlineStr">
-        <is>
-          <t>public</t>
-        </is>
-      </c>
-      <c r="F25" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G25" s="9" t="n">
-        <v>500</v>
-      </c>
-      <c r="H25" s="10" t="n">
-        <v>500</v>
-      </c>
+      <c r="E25" s="4" t="n"/>
+      <c r="F25" s="2" t="n"/>
+      <c r="G25" s="9" t="n"/>
+      <c r="H25" s="10" t="n"/>
       <c r="I25" s="16" t="n"/>
     </row>
     <row r="26" ht="16.5" customHeight="1">
@@ -1179,15 +1157,9 @@
       <c r="C26" s="29" t="n"/>
       <c r="D26" s="29" t="n"/>
       <c r="E26" s="30" t="n"/>
-      <c r="F26" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G26" s="9" t="n">
-        <v>60</v>
-      </c>
-      <c r="H26" s="10" t="n">
-        <v>60</v>
-      </c>
+      <c r="F26" s="2" t="n"/>
+      <c r="G26" s="9" t="n"/>
+      <c r="H26" s="10" t="n"/>
       <c r="I26" s="16" t="n"/>
     </row>
     <row r="27" ht="17.5" customHeight="1">
@@ -1203,20 +1175,10 @@
           <t>Period (years):</t>
         </is>
       </c>
-      <c r="E27" s="4" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="F27" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="G27" s="9" t="n">
-        <v>40</v>
-      </c>
-      <c r="H27" s="10" t="n">
-        <v>25000</v>
-      </c>
+      <c r="E27" s="4" t="n"/>
+      <c r="F27" s="2" t="n"/>
+      <c r="G27" s="9" t="n"/>
+      <c r="H27" s="10" t="n"/>
       <c r="I27" s="16" t="n"/>
     </row>
     <row r="28">
@@ -1244,15 +1206,9 @@
       <c r="C29" s="29" t="n"/>
       <c r="D29" s="29" t="n"/>
       <c r="E29" s="30" t="n"/>
-      <c r="F29" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="9" t="n">
-        <v>79900</v>
-      </c>
-      <c r="H29" s="10" t="n">
-        <v>79900</v>
-      </c>
+      <c r="F29" s="2" t="n"/>
+      <c r="G29" s="9" t="n"/>
+      <c r="H29" s="10" t="n"/>
       <c r="I29" s="16" t="n"/>
     </row>
     <row r="30" ht="17.25" customHeight="1">
@@ -1265,15 +1221,9 @@
       <c r="C30" s="29" t="n"/>
       <c r="D30" s="29" t="n"/>
       <c r="E30" s="30" t="n"/>
-      <c r="F30" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="9" t="n">
-        <v>3000</v>
-      </c>
-      <c r="H30" s="10" t="n">
-        <v>3000</v>
-      </c>
+      <c r="F30" s="2" t="n"/>
+      <c r="G30" s="9" t="n"/>
+      <c r="H30" s="10" t="n"/>
       <c r="I30" s="16" t="n"/>
     </row>
     <row r="31">
@@ -1289,20 +1239,10 @@
           <t>Type:</t>
         </is>
       </c>
-      <c r="E31" s="6" t="inlineStr">
-        <is>
-          <t>gold</t>
-        </is>
-      </c>
-      <c r="F31" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G31" s="9" t="n">
-        <v>2500</v>
-      </c>
-      <c r="H31" s="10" t="n">
-        <v>2500</v>
-      </c>
+      <c r="E31" s="6" t="n"/>
+      <c r="F31" s="2" t="n"/>
+      <c r="G31" s="9" t="n"/>
+      <c r="H31" s="10" t="n"/>
       <c r="I31" s="16" t="n"/>
     </row>
     <row r="32">
@@ -1319,14 +1259,14 @@
         </is>
       </c>
       <c r="E32" s="6" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="F32" s="2" t="n"/>
       <c r="G32" s="9" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H32" s="10" t="n">
-        <v>500</v>
+        <v>60</v>
       </c>
       <c r="I32" s="16" t="n"/>
     </row>
@@ -1338,7 +1278,7 @@
         </is>
       </c>
       <c r="H33" s="12" t="n">
-        <v>162952</v>
+        <v>3510</v>
       </c>
     </row>
     <row r="34">
@@ -1352,7 +1292,7 @@
       <c r="F34" s="47" t="n"/>
       <c r="G34" s="48" t="n"/>
       <c r="H34" s="13" t="n">
-        <v>12532</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">

</xml_diff>

<commit_message>
add partner name to the order form
</commit_message>
<xml_diff>
--- a/calc/static/calc/Piql_order_form.xlsx
+++ b/calc/static/calc/Piql_order_form.xlsx
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="G4" s="25" t="n">
-        <v>44079.51026330685</v>
+        <v>44079.5792554584</v>
       </c>
     </row>
     <row r="5" ht="14.15" customHeight="1">
@@ -852,7 +852,11 @@
           <t>Piql Partner:</t>
         </is>
       </c>
-      <c r="G5" s="26" t="n"/>
+      <c r="G5" s="26" t="inlineStr">
+        <is>
+          <t>alfrtruj</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="14.15" customHeight="1">
       <c r="A6" s="26" t="n"/>
@@ -872,7 +876,7 @@
       </c>
       <c r="G7" s="26" t="inlineStr">
         <is>
-          <t>Unesco</t>
+          <t>El enano</t>
         </is>
       </c>
     </row>
@@ -909,7 +913,7 @@
       <c r="E10" s="48" t="n"/>
       <c r="F10" s="36" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>el perro</t>
         </is>
       </c>
       <c r="H10" s="34" t="n"/>
@@ -1010,15 +1014,9 @@
       <c r="C18" s="29" t="n"/>
       <c r="D18" s="29" t="n"/>
       <c r="E18" s="30" t="n"/>
-      <c r="F18" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G18" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="H18" s="10" t="n">
-        <v>1500</v>
-      </c>
+      <c r="F18" s="2" t="n"/>
+      <c r="G18" s="9" t="n"/>
+      <c r="H18" s="10" t="n"/>
     </row>
     <row r="19" ht="17.25" customHeight="1">
       <c r="A19" s="32" t="inlineStr">
@@ -1030,9 +1028,15 @@
       <c r="C19" s="29" t="n"/>
       <c r="D19" s="29" t="n"/>
       <c r="E19" s="30" t="n"/>
-      <c r="F19" s="14" t="n"/>
-      <c r="G19" s="9" t="n"/>
-      <c r="H19" s="10" t="n"/>
+      <c r="F19" s="14" t="n">
+        <v>450</v>
+      </c>
+      <c r="G19" s="9" t="n">
+        <v>15</v>
+      </c>
+      <c r="H19" s="10" t="n">
+        <v>4950</v>
+      </c>
       <c r="I19" s="16" t="n"/>
     </row>
     <row r="20" ht="17.25" customHeight="1">
@@ -1048,20 +1052,10 @@
           <t>Pages/frame:</t>
         </is>
       </c>
-      <c r="E20" s="8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F20" s="15" t="n">
-        <v>67000</v>
-      </c>
-      <c r="G20" s="11" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="H20" s="10" t="n">
-        <v>2010</v>
-      </c>
+      <c r="E20" s="8" t="n"/>
+      <c r="F20" s="15" t="n"/>
+      <c r="G20" s="11" t="n"/>
+      <c r="H20" s="10" t="n"/>
       <c r="I20" s="16" t="n"/>
     </row>
     <row r="21" ht="17.25" customHeight="1">
@@ -1074,9 +1068,15 @@
       <c r="C21" s="29" t="n"/>
       <c r="D21" s="29" t="n"/>
       <c r="E21" s="30" t="n"/>
-      <c r="F21" s="2" t="n"/>
-      <c r="G21" s="9" t="n"/>
-      <c r="H21" s="10" t="n"/>
+      <c r="F21" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="9" t="n">
+        <v>8880</v>
+      </c>
+      <c r="H21" s="10" t="n">
+        <v>8880</v>
+      </c>
       <c r="I21" s="16" t="n"/>
     </row>
     <row r="22" ht="17.25" customHeight="1">
@@ -1092,10 +1092,20 @@
           <t>Payment:</t>
         </is>
       </c>
-      <c r="E22" s="4" t="n"/>
-      <c r="F22" s="2" t="n"/>
-      <c r="G22" s="11" t="n"/>
-      <c r="H22" s="10" t="n"/>
+      <c r="E22" s="4" t="inlineStr">
+        <is>
+          <t>yearly</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>7890</v>
+      </c>
+      <c r="G22" s="11" t="n">
+        <v>0.576</v>
+      </c>
+      <c r="H22" s="10" t="n">
+        <v>3968.64</v>
+      </c>
       <c r="I22" s="16" t="n"/>
     </row>
     <row r="23" ht="17.25" customHeight="1">
@@ -1259,14 +1269,14 @@
         </is>
       </c>
       <c r="E32" s="6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F32" s="2" t="n"/>
       <c r="G32" s="9" t="n">
         <v>30</v>
       </c>
       <c r="H32" s="10" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="I32" s="16" t="n"/>
     </row>
@@ -1278,7 +1288,7 @@
         </is>
       </c>
       <c r="H33" s="12" t="n">
-        <v>3510</v>
+        <v>17798.64</v>
       </c>
     </row>
     <row r="34">
@@ -1292,7 +1302,7 @@
       <c r="F34" s="47" t="n"/>
       <c r="G34" s="48" t="n"/>
       <c r="H34" s="13" t="n">
-        <v>0</v>
+        <v>12848.64</v>
       </c>
     </row>
     <row r="35">

</xml_diff>

<commit_message>
fix free reel option when hybrid and online request.
</commit_message>
<xml_diff>
--- a/calc/static/calc/Piql_order_form.xlsx
+++ b/calc/static/calc/Piql_order_form.xlsx
@@ -802,7 +802,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScale="96" zoomScaleNormal="55" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="16.5"/>
@@ -816,8 +816,8 @@
     <col width="11.54296875" bestFit="1" customWidth="1" style="22" min="7" max="7"/>
     <col width="14" customWidth="1" style="22" min="8" max="8"/>
     <col width="10.453125" customWidth="1" style="22" min="9" max="9"/>
-    <col width="9.1796875" customWidth="1" style="22" min="10" max="41"/>
-    <col width="9.1796875" customWidth="1" style="22" min="42" max="16384"/>
+    <col width="9.1796875" customWidth="1" style="22" min="10" max="43"/>
+    <col width="9.1796875" customWidth="1" style="22" min="44" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="G4" s="25" t="n">
-        <v>44079.5792554584</v>
+        <v>44080.31259962761</v>
       </c>
     </row>
     <row r="5" ht="14.15" customHeight="1">
@@ -876,7 +876,7 @@
       </c>
       <c r="G7" s="26" t="inlineStr">
         <is>
-          <t>El enano</t>
+          <t>El popeye</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       <c r="E10" s="48" t="n"/>
       <c r="F10" s="36" t="inlineStr">
         <is>
-          <t>el perro</t>
+          <t>Camisetas el chamin</t>
         </is>
       </c>
       <c r="H10" s="34" t="n"/>
@@ -1029,13 +1029,13 @@
       <c r="D19" s="29" t="n"/>
       <c r="E19" s="30" t="n"/>
       <c r="F19" s="14" t="n">
-        <v>450</v>
+        <v>670</v>
       </c>
       <c r="G19" s="9" t="n">
         <v>15</v>
       </c>
       <c r="H19" s="10" t="n">
-        <v>4950</v>
+        <v>8250</v>
       </c>
       <c r="I19" s="16" t="n"/>
     </row>
@@ -1098,13 +1098,13 @@
         </is>
       </c>
       <c r="F22" s="2" t="n">
-        <v>7890</v>
+        <v>8000</v>
       </c>
       <c r="G22" s="11" t="n">
         <v>0.576</v>
       </c>
       <c r="H22" s="10" t="n">
-        <v>3968.64</v>
+        <v>4032</v>
       </c>
       <c r="I22" s="16" t="n"/>
     </row>
@@ -1269,14 +1269,14 @@
         </is>
       </c>
       <c r="E32" s="6" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F32" s="2" t="n"/>
       <c r="G32" s="9" t="n">
         <v>30</v>
       </c>
       <c r="H32" s="10" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="I32" s="16" t="n"/>
     </row>
@@ -1288,7 +1288,7 @@
         </is>
       </c>
       <c r="H33" s="12" t="n">
-        <v>17798.64</v>
+        <v>21162</v>
       </c>
     </row>
     <row r="34">
@@ -1302,7 +1302,7 @@
       <c r="F34" s="47" t="n"/>
       <c r="G34" s="48" t="n"/>
       <c r="H34" s="13" t="n">
-        <v>12848.64</v>
+        <v>12912</v>
       </c>
     </row>
     <row r="35">

</xml_diff>

<commit_message>
solved disabling fields according to other field inputs.
</commit_message>
<xml_diff>
--- a/calc/static/calc/Piql_order_form.xlsx
+++ b/calc/static/calc/Piql_order_form.xlsx
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="G4" s="59" t="n">
-        <v>44080.39421688148</v>
+        <v>44080.8674935521</v>
       </c>
     </row>
     <row r="5" ht="14.15" customHeight="1">
@@ -876,7 +876,7 @@
       </c>
       <c r="G7" s="23" t="inlineStr">
         <is>
-          <t>Camino Real LTDA</t>
+          <t>El caballo vengador</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       <c r="E10" s="42" t="n"/>
       <c r="F10" s="45" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>Tirando las maletas</t>
         </is>
       </c>
       <c r="H10" s="28" t="n"/>
@@ -1014,9 +1014,15 @@
       <c r="C18" s="25" t="n"/>
       <c r="D18" s="25" t="n"/>
       <c r="E18" s="34" t="n"/>
-      <c r="F18" s="2" t="n"/>
-      <c r="G18" s="9" t="n"/>
-      <c r="H18" s="10" t="n"/>
+      <c r="F18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="9" t="n">
+        <v>1500</v>
+      </c>
+      <c r="H18" s="10" t="n">
+        <v>1500</v>
+      </c>
     </row>
     <row r="19" ht="17.25" customHeight="1">
       <c r="A19" s="36" t="inlineStr">
@@ -1029,13 +1035,13 @@
       <c r="D19" s="25" t="n"/>
       <c r="E19" s="34" t="n"/>
       <c r="F19" s="14" t="n">
-        <v>789</v>
+        <v>450</v>
       </c>
       <c r="G19" s="9" t="n">
         <v>15</v>
       </c>
       <c r="H19" s="10" t="n">
-        <v>10035</v>
+        <v>6750</v>
       </c>
       <c r="I19" s="16" t="n"/>
     </row>
@@ -1068,15 +1074,9 @@
       <c r="C21" s="25" t="n"/>
       <c r="D21" s="25" t="n"/>
       <c r="E21" s="34" t="n"/>
-      <c r="F21" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="9" t="n">
-        <v>8880</v>
-      </c>
-      <c r="H21" s="10" t="n">
-        <v>8880</v>
-      </c>
+      <c r="F21" s="2" t="n"/>
+      <c r="G21" s="9" t="n"/>
+      <c r="H21" s="10" t="n"/>
       <c r="I21" s="16" t="n"/>
     </row>
     <row r="22" ht="17.25" customHeight="1">
@@ -1092,20 +1092,10 @@
           <t>Payment:</t>
         </is>
       </c>
-      <c r="E22" s="4" t="inlineStr">
-        <is>
-          <t>yearly</t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="G22" s="11" t="n">
-        <v>0.576</v>
-      </c>
-      <c r="H22" s="10" t="n">
-        <v>576</v>
-      </c>
+      <c r="E22" s="4" t="n"/>
+      <c r="F22" s="2" t="n"/>
+      <c r="G22" s="11" t="n"/>
+      <c r="H22" s="10" t="n"/>
       <c r="I22" s="16" t="n"/>
     </row>
     <row r="23" ht="17.25" customHeight="1">
@@ -1133,15 +1123,9 @@
       <c r="C24" s="25" t="n"/>
       <c r="D24" s="25" t="n"/>
       <c r="E24" s="34" t="n"/>
-      <c r="F24" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G24" s="9" t="n">
-        <v>200</v>
-      </c>
-      <c r="H24" s="10" t="n">
-        <v>200</v>
-      </c>
+      <c r="F24" s="2" t="n"/>
+      <c r="G24" s="9" t="n"/>
+      <c r="H24" s="10" t="n"/>
       <c r="I24" s="16" t="n"/>
     </row>
     <row r="25" ht="16.5" customHeight="1">
@@ -1157,20 +1141,10 @@
           <t>Entity:</t>
         </is>
       </c>
-      <c r="E25" s="4" t="inlineStr">
-        <is>
-          <t>public</t>
-        </is>
-      </c>
-      <c r="F25" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G25" s="9" t="n">
-        <v>500</v>
-      </c>
-      <c r="H25" s="10" t="n">
-        <v>500</v>
-      </c>
+      <c r="E25" s="4" t="n"/>
+      <c r="F25" s="2" t="n"/>
+      <c r="G25" s="9" t="n"/>
+      <c r="H25" s="10" t="n"/>
       <c r="I25" s="16" t="n"/>
     </row>
     <row r="26" ht="16.5" customHeight="1">
@@ -1183,15 +1157,9 @@
       <c r="C26" s="25" t="n"/>
       <c r="D26" s="25" t="n"/>
       <c r="E26" s="34" t="n"/>
-      <c r="F26" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G26" s="9" t="n">
-        <v>60</v>
-      </c>
-      <c r="H26" s="10" t="n">
-        <v>600</v>
-      </c>
+      <c r="F26" s="2" t="n"/>
+      <c r="G26" s="9" t="n"/>
+      <c r="H26" s="10" t="n"/>
       <c r="I26" s="16" t="n"/>
     </row>
     <row r="27" ht="17.5" customHeight="1">
@@ -1207,20 +1175,10 @@
           <t>Period (years):</t>
         </is>
       </c>
-      <c r="E27" s="4" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F27" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="G27" s="9" t="n">
-        <v>48</v>
-      </c>
-      <c r="H27" s="10" t="n">
-        <v>3360</v>
-      </c>
+      <c r="E27" s="4" t="n"/>
+      <c r="F27" s="2" t="n"/>
+      <c r="G27" s="9" t="n"/>
+      <c r="H27" s="10" t="n"/>
       <c r="I27" s="16" t="n"/>
     </row>
     <row r="28">
@@ -1233,15 +1191,9 @@
       <c r="C28" s="25" t="n"/>
       <c r="D28" s="25" t="n"/>
       <c r="E28" s="34" t="n"/>
-      <c r="F28" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" s="9" t="n">
-        <v>900</v>
-      </c>
-      <c r="H28" s="10" t="n">
-        <v>900</v>
-      </c>
+      <c r="F28" s="2" t="n"/>
+      <c r="G28" s="9" t="n"/>
+      <c r="H28" s="10" t="n"/>
       <c r="I28" s="16" t="n"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
@@ -1254,15 +1206,9 @@
       <c r="C29" s="25" t="n"/>
       <c r="D29" s="25" t="n"/>
       <c r="E29" s="34" t="n"/>
-      <c r="F29" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="9" t="n">
-        <v>79900</v>
-      </c>
-      <c r="H29" s="10" t="n">
-        <v>79900</v>
-      </c>
+      <c r="F29" s="2" t="n"/>
+      <c r="G29" s="9" t="n"/>
+      <c r="H29" s="10" t="n"/>
       <c r="I29" s="16" t="n"/>
     </row>
     <row r="30" ht="17.25" customHeight="1">
@@ -1275,15 +1221,9 @@
       <c r="C30" s="25" t="n"/>
       <c r="D30" s="25" t="n"/>
       <c r="E30" s="34" t="n"/>
-      <c r="F30" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="9" t="n">
-        <v>3000</v>
-      </c>
-      <c r="H30" s="10" t="n">
-        <v>3000</v>
-      </c>
+      <c r="F30" s="2" t="n"/>
+      <c r="G30" s="9" t="n"/>
+      <c r="H30" s="10" t="n"/>
       <c r="I30" s="16" t="n"/>
     </row>
     <row r="31">
@@ -1299,20 +1239,10 @@
           <t>Type:</t>
         </is>
       </c>
-      <c r="E31" s="6" t="inlineStr">
-        <is>
-          <t>gold</t>
-        </is>
-      </c>
-      <c r="F31" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G31" s="9" t="n">
-        <v>2500</v>
-      </c>
-      <c r="H31" s="10" t="n">
-        <v>2500</v>
-      </c>
+      <c r="E31" s="6" t="n"/>
+      <c r="F31" s="2" t="n"/>
+      <c r="G31" s="9" t="n"/>
+      <c r="H31" s="10" t="n"/>
       <c r="I31" s="16" t="n"/>
     </row>
     <row r="32">
@@ -1329,14 +1259,14 @@
         </is>
       </c>
       <c r="E32" s="6" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F32" s="2" t="n"/>
       <c r="G32" s="9" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H32" s="10" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="I32" s="16" t="n"/>
     </row>
@@ -1348,7 +1278,7 @@
         </is>
       </c>
       <c r="H33" s="12" t="n">
-        <v>110451</v>
+        <v>8250</v>
       </c>
     </row>
     <row r="34">
@@ -1362,7 +1292,7 @@
       <c r="F34" s="41" t="n"/>
       <c r="G34" s="42" t="n"/>
       <c r="H34" s="13" t="n">
-        <v>11956</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">

</xml_diff>

<commit_message>
including shipment cost in order form
</commit_message>
<xml_diff>
--- a/calc/static/calc/Piql_order_form.xlsx
+++ b/calc/static/calc/Piql_order_form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="order" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <numFmt numFmtId="165" formatCode="_-[$€-2]\ * #,##0.000_-;\-[$€-2]\ * #,##0.000_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -100,14 +100,6 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="10"/>
-      <sz val="7"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <color theme="1"/>
       <sz val="9"/>
       <scheme val="minor"/>
@@ -312,7 +304,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
@@ -329,13 +321,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
@@ -361,74 +353,57 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -437,22 +412,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -801,8 +792,8 @@
   </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="96" zoomScaleNormal="55" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScale="96" zoomScaleNormal="55" zoomScalePageLayoutView="96" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="16.5"/>
@@ -816,165 +807,165 @@
     <col width="11.54296875" bestFit="1" customWidth="1" style="22" min="7" max="7"/>
     <col width="14" customWidth="1" style="22" min="8" max="8"/>
     <col width="11.26953125" bestFit="1" customWidth="1" style="22" min="9" max="9"/>
-    <col width="9.1796875" customWidth="1" style="22" min="10" max="46"/>
-    <col width="9.1796875" customWidth="1" style="22" min="47" max="16384"/>
+    <col width="9.1796875" customWidth="1" style="22" min="10" max="47"/>
+    <col width="9.1796875" customWidth="1" style="22" min="48" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
-      <c r="A1" s="23" t="n"/>
-      <c r="E1" s="56" t="inlineStr">
+      <c r="A1" s="26" t="n"/>
+      <c r="E1" s="21" t="inlineStr">
         <is>
           <t>Partner Order Form</t>
         </is>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
-      <c r="A2" s="23" t="n"/>
+      <c r="A2" s="26" t="n"/>
     </row>
     <row r="3" ht="14.15" customHeight="1">
-      <c r="A3" s="48" t="n"/>
+      <c r="A3" s="41" t="n"/>
     </row>
     <row r="4" ht="14.15" customHeight="1">
-      <c r="A4" s="23" t="n"/>
-      <c r="E4" s="57" t="inlineStr">
+      <c r="A4" s="26" t="n"/>
+      <c r="E4" s="23" t="inlineStr">
         <is>
           <t>Date:</t>
         </is>
       </c>
-      <c r="G4" s="59" t="n">
-        <v>44080.87444465241</v>
+      <c r="G4" s="25" t="n">
+        <v>44090.44160509142</v>
       </c>
     </row>
     <row r="5" ht="14.15" customHeight="1">
-      <c r="A5" s="23" t="n"/>
-      <c r="E5" s="57" t="inlineStr">
+      <c r="A5" s="26" t="n"/>
+      <c r="E5" s="23" t="inlineStr">
         <is>
           <t>Piql Partner:</t>
         </is>
       </c>
-      <c r="G5" s="23" t="inlineStr">
+      <c r="G5" s="26" t="inlineStr">
         <is>
           <t>alfrtruj</t>
         </is>
       </c>
     </row>
     <row r="6" ht="14.15" customHeight="1">
-      <c r="A6" s="23" t="n"/>
-      <c r="E6" s="57" t="inlineStr">
+      <c r="A6" s="26" t="n"/>
+      <c r="E6" s="23" t="inlineStr">
         <is>
           <t>Partner Order Number:</t>
         </is>
       </c>
-      <c r="G6" s="60" t="n"/>
+      <c r="G6" s="27" t="n"/>
     </row>
     <row r="7" ht="14.15" customHeight="1">
-      <c r="A7" s="23" t="n"/>
-      <c r="E7" s="58" t="inlineStr">
+      <c r="A7" s="26" t="n"/>
+      <c r="E7" s="24" t="inlineStr">
         <is>
           <t>Customer name:</t>
         </is>
       </c>
-      <c r="G7" s="23" t="inlineStr">
-        <is>
-          <t>Trujillo AS</t>
+      <c r="G7" s="26" t="inlineStr">
+        <is>
+          <t>Kuben</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="23" t="n"/>
+      <c r="A8" s="26" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="44" t="inlineStr">
+      <c r="A9" s="28" t="inlineStr">
         <is>
           <t>PIQL PARTNER &lt;Mandatory&gt;</t>
         </is>
       </c>
-      <c r="B9" s="25" t="n"/>
-      <c r="C9" s="25" t="n"/>
-      <c r="D9" s="25" t="n"/>
-      <c r="E9" s="34" t="n"/>
-      <c r="F9" s="44" t="inlineStr">
+      <c r="B9" s="29" t="n"/>
+      <c r="C9" s="29" t="n"/>
+      <c r="D9" s="29" t="n"/>
+      <c r="E9" s="30" t="n"/>
+      <c r="F9" s="28" t="inlineStr">
         <is>
           <t>Comments:</t>
         </is>
       </c>
-      <c r="G9" s="25" t="n"/>
-      <c r="H9" s="34" t="n"/>
+      <c r="G9" s="29" t="n"/>
+      <c r="H9" s="30" t="n"/>
     </row>
     <row r="10" ht="17.25" customHeight="1">
-      <c r="A10" s="53" t="inlineStr">
+      <c r="A10" s="46" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="B10" s="41" t="n"/>
-      <c r="C10" s="41" t="n"/>
-      <c r="D10" s="41" t="n"/>
-      <c r="E10" s="42" t="n"/>
-      <c r="F10" s="45" t="inlineStr">
-        <is>
-          <t>El texto</t>
-        </is>
-      </c>
-      <c r="H10" s="28" t="n"/>
+      <c r="B10" s="47" t="n"/>
+      <c r="C10" s="47" t="n"/>
+      <c r="D10" s="47" t="n"/>
+      <c r="E10" s="48" t="n"/>
+      <c r="F10" s="36" t="inlineStr">
+        <is>
+          <t>Comments about the job, logistics, shipment address (client contact details), special considerations, etc</t>
+        </is>
+      </c>
+      <c r="H10" s="34" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="27" t="inlineStr">
+      <c r="A11" s="33" t="inlineStr">
         <is>
           <t>Contact person</t>
         </is>
       </c>
-      <c r="E11" s="28" t="n"/>
-      <c r="F11" s="46" t="n"/>
-      <c r="H11" s="28" t="n"/>
+      <c r="E11" s="34" t="n"/>
+      <c r="F11" s="37" t="n"/>
+      <c r="H11" s="34" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="29" t="inlineStr">
+      <c r="A12" s="57" t="inlineStr">
         <is>
           <t>Telephone</t>
         </is>
       </c>
-      <c r="E12" s="28" t="n"/>
-      <c r="F12" s="46" t="n"/>
-      <c r="H12" s="28" t="n"/>
+      <c r="E12" s="34" t="n"/>
+      <c r="F12" s="37" t="n"/>
+      <c r="H12" s="34" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="29" t="inlineStr">
+      <c r="A13" s="57" t="inlineStr">
         <is>
           <t>email:</t>
         </is>
       </c>
-      <c r="E13" s="28" t="n"/>
-      <c r="F13" s="46" t="n"/>
-      <c r="H13" s="28" t="n"/>
+      <c r="E13" s="34" t="n"/>
+      <c r="F13" s="37" t="n"/>
+      <c r="H13" s="34" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="27" t="n"/>
-      <c r="E14" s="28" t="n"/>
-      <c r="F14" s="46" t="n"/>
-      <c r="H14" s="28" t="n"/>
+      <c r="A14" s="33" t="n"/>
+      <c r="E14" s="34" t="n"/>
+      <c r="F14" s="37" t="n"/>
+      <c r="H14" s="34" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="30" t="n"/>
-      <c r="B15" s="31" t="n"/>
-      <c r="C15" s="31" t="n"/>
-      <c r="D15" s="31" t="n"/>
-      <c r="E15" s="32" t="n"/>
-      <c r="F15" s="47" t="n"/>
-      <c r="G15" s="31" t="n"/>
-      <c r="H15" s="32" t="n"/>
+      <c r="A15" s="58" t="n"/>
+      <c r="B15" s="39" t="n"/>
+      <c r="C15" s="39" t="n"/>
+      <c r="D15" s="39" t="n"/>
+      <c r="E15" s="40" t="n"/>
+      <c r="F15" s="38" t="n"/>
+      <c r="G15" s="39" t="n"/>
+      <c r="H15" s="40" t="n"/>
     </row>
     <row r="16" ht="30" customHeight="1">
-      <c r="A16" s="33" t="inlineStr">
+      <c r="A16" s="59" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="B16" s="25" t="n"/>
-      <c r="C16" s="25" t="n"/>
-      <c r="D16" s="25" t="n"/>
-      <c r="E16" s="34" t="n"/>
-      <c r="F16" s="33" t="inlineStr">
+      <c r="B16" s="29" t="n"/>
+      <c r="C16" s="29" t="n"/>
+      <c r="D16" s="29" t="n"/>
+      <c r="E16" s="30" t="n"/>
+      <c r="F16" s="59" t="inlineStr">
         <is>
           <t>Qty</t>
         </is>
@@ -996,51 +987,57 @@
           <t>1. Offline Storage (one-off payment)</t>
         </is>
       </c>
-      <c r="B17" s="25" t="n"/>
-      <c r="C17" s="25" t="n"/>
-      <c r="D17" s="25" t="n"/>
-      <c r="E17" s="34" t="n"/>
+      <c r="B17" s="29" t="n"/>
+      <c r="C17" s="29" t="n"/>
+      <c r="D17" s="29" t="n"/>
+      <c r="E17" s="30" t="n"/>
       <c r="F17" s="2" t="n"/>
       <c r="G17" s="9" t="n"/>
       <c r="H17" s="10" t="n"/>
     </row>
     <row r="18" ht="16.5" customHeight="1">
-      <c r="A18" s="36" t="inlineStr">
+      <c r="A18" s="32" t="inlineStr">
         <is>
           <t>piqlConnect (only piqlFilm)</t>
         </is>
       </c>
-      <c r="B18" s="25" t="n"/>
-      <c r="C18" s="25" t="n"/>
-      <c r="D18" s="25" t="n"/>
-      <c r="E18" s="34" t="n"/>
+      <c r="B18" s="29" t="n"/>
+      <c r="C18" s="29" t="n"/>
+      <c r="D18" s="29" t="n"/>
+      <c r="E18" s="30" t="n"/>
       <c r="F18" s="2" t="n"/>
       <c r="G18" s="9" t="n"/>
       <c r="H18" s="10" t="n"/>
     </row>
     <row r="19" ht="17.25" customHeight="1">
-      <c r="A19" s="36" t="inlineStr">
+      <c r="A19" s="32" t="inlineStr">
         <is>
           <t>Digital (GB)</t>
         </is>
       </c>
-      <c r="B19" s="25" t="n"/>
-      <c r="C19" s="25" t="n"/>
-      <c r="D19" s="25" t="n"/>
-      <c r="E19" s="34" t="n"/>
-      <c r="F19" s="14" t="n"/>
-      <c r="G19" s="9" t="n"/>
-      <c r="H19" s="10" t="n"/>
+      <c r="B19" s="29" t="n"/>
+      <c r="C19" s="29" t="n"/>
+      <c r="D19" s="29" t="n"/>
+      <c r="E19" s="30" t="n"/>
+      <c r="F19" s="14" t="n">
+        <v>360</v>
+      </c>
+      <c r="G19" s="9" t="n">
+        <v>15</v>
+      </c>
+      <c r="H19" s="10" t="n">
+        <v>3600</v>
+      </c>
       <c r="I19" s="16" t="n"/>
     </row>
     <row r="20" ht="17.25" customHeight="1">
-      <c r="A20" s="37" t="inlineStr">
+      <c r="A20" s="31" t="inlineStr">
         <is>
           <t>Visual (pages)</t>
         </is>
       </c>
-      <c r="B20" s="25" t="n"/>
-      <c r="C20" s="25" t="n"/>
+      <c r="B20" s="29" t="n"/>
+      <c r="C20" s="29" t="n"/>
       <c r="D20" s="7" t="inlineStr">
         <is>
           <t>Pages/frame:</t>
@@ -1052,13 +1049,13 @@
         </is>
       </c>
       <c r="F20" s="15" t="n">
-        <v>89000</v>
+        <v>130000</v>
       </c>
       <c r="G20" s="11" t="n">
         <v>0.03</v>
       </c>
       <c r="H20" s="10" t="n">
-        <v>720</v>
+        <v>3900</v>
       </c>
       <c r="I20" s="16" t="n"/>
     </row>
@@ -1068,10 +1065,10 @@
           <t>2. Online Storage (GB) - piqlConnect (1 TB &amp; 1 piqlFilm included)</t>
         </is>
       </c>
-      <c r="B21" s="25" t="n"/>
-      <c r="C21" s="25" t="n"/>
-      <c r="D21" s="25" t="n"/>
-      <c r="E21" s="34" t="n"/>
+      <c r="B21" s="29" t="n"/>
+      <c r="C21" s="29" t="n"/>
+      <c r="D21" s="29" t="n"/>
+      <c r="E21" s="30" t="n"/>
       <c r="F21" s="2" t="n">
         <v>1</v>
       </c>
@@ -1084,13 +1081,13 @@
       <c r="I21" s="16" t="n"/>
     </row>
     <row r="22" ht="17.25" customHeight="1">
-      <c r="A22" s="37" t="inlineStr">
+      <c r="A22" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Online Storage (GB) </t>
         </is>
       </c>
-      <c r="B22" s="25" t="n"/>
-      <c r="C22" s="25" t="n"/>
+      <c r="B22" s="29" t="n"/>
+      <c r="C22" s="29" t="n"/>
       <c r="D22" s="3" t="inlineStr">
         <is>
           <t>Payment:</t>
@@ -1102,13 +1099,13 @@
         </is>
       </c>
       <c r="F22" s="2" t="n">
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="G22" s="11" t="n">
         <v>0.576</v>
       </c>
       <c r="H22" s="10" t="n">
-        <v>2880</v>
+        <v>576</v>
       </c>
       <c r="I22" s="16" t="n"/>
     </row>
@@ -1118,81 +1115,115 @@
           <t xml:space="preserve">3. Arctic World Archive </t>
         </is>
       </c>
-      <c r="B23" s="25" t="n"/>
-      <c r="C23" s="25" t="n"/>
-      <c r="D23" s="25" t="n"/>
-      <c r="E23" s="34" t="n"/>
+      <c r="B23" s="29" t="n"/>
+      <c r="C23" s="29" t="n"/>
+      <c r="D23" s="29" t="n"/>
+      <c r="E23" s="30" t="n"/>
       <c r="F23" s="2" t="n"/>
       <c r="G23" s="9" t="n"/>
       <c r="H23" s="10" t="n"/>
       <c r="I23" s="16" t="n"/>
     </row>
     <row r="24" ht="16.5" customHeight="1">
-      <c r="A24" s="36" t="inlineStr">
+      <c r="A24" s="32" t="inlineStr">
         <is>
           <t>Registration fee</t>
         </is>
       </c>
-      <c r="B24" s="25" t="n"/>
-      <c r="C24" s="25" t="n"/>
-      <c r="D24" s="25" t="n"/>
-      <c r="E24" s="34" t="n"/>
-      <c r="F24" s="2" t="n"/>
-      <c r="G24" s="9" t="n"/>
-      <c r="H24" s="10" t="n"/>
+      <c r="B24" s="29" t="n"/>
+      <c r="C24" s="29" t="n"/>
+      <c r="D24" s="29" t="n"/>
+      <c r="E24" s="30" t="n"/>
+      <c r="F24" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" s="9" t="n">
+        <v>200</v>
+      </c>
+      <c r="H24" s="10" t="n">
+        <v>200</v>
+      </c>
       <c r="I24" s="16" t="n"/>
     </row>
     <row r="25" ht="16.5" customHeight="1">
-      <c r="A25" s="37" t="inlineStr">
+      <c r="A25" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">AWA contribution </t>
         </is>
       </c>
-      <c r="B25" s="25" t="n"/>
-      <c r="C25" s="25" t="n"/>
+      <c r="B25" s="29" t="n"/>
+      <c r="C25" s="29" t="n"/>
       <c r="D25" s="3" t="inlineStr">
         <is>
           <t>Entity:</t>
         </is>
       </c>
-      <c r="E25" s="4" t="n"/>
-      <c r="F25" s="2" t="n"/>
-      <c r="G25" s="9" t="n"/>
-      <c r="H25" s="10" t="n"/>
+      <c r="E25" s="4" t="inlineStr">
+        <is>
+          <t>public</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="9" t="n">
+        <v>500</v>
+      </c>
+      <c r="H25" s="10" t="n">
+        <v>500</v>
+      </c>
       <c r="I25" s="16" t="n"/>
     </row>
     <row r="26" ht="16.5" customHeight="1">
-      <c r="A26" s="36" t="inlineStr">
+      <c r="A26" s="32" t="inlineStr">
         <is>
           <t>Management fee (per period)</t>
         </is>
       </c>
-      <c r="B26" s="25" t="n"/>
-      <c r="C26" s="25" t="n"/>
-      <c r="D26" s="25" t="n"/>
-      <c r="E26" s="34" t="n"/>
-      <c r="F26" s="2" t="n"/>
-      <c r="G26" s="9" t="n"/>
-      <c r="H26" s="10" t="n"/>
+      <c r="B26" s="29" t="n"/>
+      <c r="C26" s="29" t="n"/>
+      <c r="D26" s="29" t="n"/>
+      <c r="E26" s="30" t="n"/>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G26" s="9" t="n">
+        <v>60</v>
+      </c>
+      <c r="H26" s="10" t="n">
+        <v>300</v>
+      </c>
       <c r="I26" s="16" t="n"/>
     </row>
     <row r="27" ht="17.5" customHeight="1">
-      <c r="A27" s="37" t="inlineStr">
+      <c r="A27" s="31" t="inlineStr">
         <is>
           <t>Storage (per reel / per period)</t>
         </is>
       </c>
-      <c r="B27" s="25" t="n"/>
-      <c r="C27" s="25" t="n"/>
+      <c r="B27" s="29" t="n"/>
+      <c r="C27" s="29" t="n"/>
       <c r="D27" s="3" t="inlineStr">
         <is>
           <t>Period (years):</t>
         </is>
       </c>
-      <c r="E27" s="4" t="n"/>
-      <c r="F27" s="2" t="n"/>
-      <c r="G27" s="9" t="n"/>
-      <c r="H27" s="10" t="n"/>
+      <c r="E27" s="4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G27" s="9" t="n">
+        <v>60</v>
+      </c>
+      <c r="H27" s="10" t="n">
+        <v>1500</v>
+      </c>
       <c r="I27" s="16" t="n"/>
     </row>
     <row r="28">
@@ -1201,13 +1232,19 @@
           <t>4. Professional Services (per day)</t>
         </is>
       </c>
-      <c r="B28" s="25" t="n"/>
-      <c r="C28" s="25" t="n"/>
-      <c r="D28" s="25" t="n"/>
-      <c r="E28" s="34" t="n"/>
-      <c r="F28" s="2" t="n"/>
-      <c r="G28" s="9" t="n"/>
-      <c r="H28" s="10" t="n"/>
+      <c r="B28" s="29" t="n"/>
+      <c r="C28" s="29" t="n"/>
+      <c r="D28" s="29" t="n"/>
+      <c r="E28" s="30" t="n"/>
+      <c r="F28" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="9" t="n">
+        <v>900</v>
+      </c>
+      <c r="H28" s="10" t="n">
+        <v>900</v>
+      </c>
       <c r="I28" s="16" t="n"/>
     </row>
     <row r="29" ht="15.5" customHeight="1">
@@ -1216,10 +1253,10 @@
           <t xml:space="preserve">5. piqlReader </t>
         </is>
       </c>
-      <c r="B29" s="25" t="n"/>
-      <c r="C29" s="25" t="n"/>
-      <c r="D29" s="25" t="n"/>
-      <c r="E29" s="34" t="n"/>
+      <c r="B29" s="29" t="n"/>
+      <c r="C29" s="29" t="n"/>
+      <c r="D29" s="29" t="n"/>
+      <c r="E29" s="30" t="n"/>
       <c r="F29" s="2" t="n">
         <v>1</v>
       </c>
@@ -1232,15 +1269,15 @@
       <c r="I29" s="16" t="n"/>
     </row>
     <row r="30" ht="17.25" customHeight="1">
-      <c r="A30" s="36" t="inlineStr">
+      <c r="A30" s="32" t="inlineStr">
         <is>
           <t>Installation and training</t>
         </is>
       </c>
-      <c r="B30" s="25" t="n"/>
-      <c r="C30" s="25" t="n"/>
-      <c r="D30" s="25" t="n"/>
-      <c r="E30" s="34" t="n"/>
+      <c r="B30" s="29" t="n"/>
+      <c r="C30" s="29" t="n"/>
+      <c r="D30" s="29" t="n"/>
+      <c r="E30" s="30" t="n"/>
       <c r="F30" s="2" t="n">
         <v>1</v>
       </c>
@@ -1253,13 +1290,13 @@
       <c r="I30" s="16" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="26" t="inlineStr">
+      <c r="A31" s="56" t="inlineStr">
         <is>
           <t>Service agreement (per year)</t>
         </is>
       </c>
-      <c r="B31" s="25" t="n"/>
-      <c r="C31" s="25" t="n"/>
+      <c r="B31" s="29" t="n"/>
+      <c r="C31" s="29" t="n"/>
       <c r="D31" s="5" t="inlineStr">
         <is>
           <t>Type:</t>
@@ -1282,161 +1319,165 @@
       <c r="I31" s="16" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="24" t="inlineStr">
+      <c r="A32" s="55" t="inlineStr">
         <is>
           <t>6. Shipment cost</t>
         </is>
       </c>
-      <c r="B32" s="25" t="n"/>
-      <c r="C32" s="25" t="n"/>
+      <c r="B32" s="29" t="n"/>
+      <c r="C32" s="29" t="n"/>
       <c r="D32" s="5" t="inlineStr">
         <is>
           <t>Reels</t>
         </is>
       </c>
       <c r="E32" s="6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F32" s="2" t="n"/>
       <c r="G32" s="9" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H32" s="10" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="I32" s="16" t="n"/>
     </row>
     <row r="33" ht="16.5" customHeight="1">
-      <c r="A33" s="38" t="n"/>
-      <c r="G33" s="40" t="inlineStr">
+      <c r="A33" s="50" t="n"/>
+      <c r="G33" s="52" t="inlineStr">
         <is>
           <t xml:space="preserve">TOTAL </t>
         </is>
       </c>
       <c r="H33" s="12" t="n">
-        <v>97880</v>
+        <v>105856</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="43" t="n"/>
-      <c r="D34" s="28" t="n"/>
-      <c r="E34" s="40" t="inlineStr">
+      <c r="A34" s="53" t="n"/>
+      <c r="D34" s="34" t="n"/>
+      <c r="E34" s="52" t="inlineStr">
         <is>
           <t>Total to pay from the second term</t>
         </is>
       </c>
-      <c r="F34" s="41" t="n"/>
-      <c r="G34" s="42" t="n"/>
+      <c r="F34" s="47" t="n"/>
+      <c r="G34" s="48" t="n"/>
       <c r="H34" s="13" t="n">
-        <v>14260</v>
+        <v>11956</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="23" t="n"/>
+      <c r="A35" s="26" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="39" t="inlineStr">
+      <c r="A36" s="51" t="inlineStr">
         <is>
           <t>Delivery terms: three weeks after the data is received by Piql. ExWorks, Drammen.</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="21" t="inlineStr">
+      <c r="A37" s="54" t="inlineStr">
         <is>
           <t xml:space="preserve">Payment terms 100% on delivery </t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="39" t="inlineStr">
+      <c r="A38" s="51" t="inlineStr">
         <is>
           <t xml:space="preserve">Notes: To provide technical and account information to the production department. Fill out this form: </t>
         </is>
       </c>
-      <c r="B38" s="39" t="n"/>
-      <c r="C38" s="39" t="n"/>
-      <c r="D38" s="39" t="n"/>
-      <c r="E38" s="39" t="n"/>
-      <c r="F38" s="39" t="n"/>
-      <c r="G38" s="39" t="n"/>
-      <c r="H38" s="39" t="n"/>
+      <c r="B38" s="51" t="n"/>
+      <c r="C38" s="51" t="n"/>
+      <c r="D38" s="51" t="n"/>
+      <c r="E38" s="51" t="n"/>
+      <c r="F38" s="51" t="n"/>
+      <c r="G38" s="51" t="n"/>
+      <c r="H38" s="51" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="55" t="inlineStr">
-        <is>
-          <t>https://forms.office.com/Pages/ResponsePage.aspx?id=k4yqUSxZRkSwWH0R7QU1A3pm4lZOZiVDhXIaxSEWbBVUM1NPUEw3OTcwMTNLQTcwVzNNOVFST1NEOC4u</t>
+      <c r="A39" s="49" t="inlineStr">
+        <is>
+          <t>piqlFilm production form - use this online form to specify the parameters to produce piqlFilm</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="51" t="n"/>
+      <c r="A40" s="44" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="48" t="inlineStr">
+      <c r="A41" s="41" t="inlineStr">
         <is>
           <t>Send this order to orders@piql.com. If you have any questions concerning this ORDER please contact:</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="52" t="inlineStr">
+      <c r="A42" s="45" t="inlineStr">
         <is>
           <t>Espen Berge Kvam</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="54" t="inlineStr">
+      <c r="A43" s="49" t="inlineStr">
         <is>
           <t>espen.berge.kvam@piql.com</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="49" t="inlineStr">
+      <c r="A44" s="42" t="inlineStr">
         <is>
           <t>+47 94030050</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="48" t="n"/>
+      <c r="A45" s="41" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="48" t="n"/>
+      <c r="A46" s="41" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="22" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="50" t="n"/>
+      <c r="A48" s="43" t="n"/>
     </row>
     <row r="49">
       <c r="A49" s="22" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="E1:H2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="A34:D34"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F10:H15"/>
     <mergeCell ref="A3:H3"/>
@@ -1453,33 +1494,29 @@
     <mergeCell ref="A45:H45"/>
     <mergeCell ref="A46:H46"/>
     <mergeCell ref="A39:H39"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E1:H2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A39" r:id="rId1"/>
+    <hyperlink ref="A39" display="piqlFilm production form - use this online form to specify the parameters to produce piqlFilm" r:id="rId1"/>
     <hyperlink ref="A43" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.46875" top="0.4791666666666667" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added download order form feature
</commit_message>
<xml_diff>
--- a/calc/static/calc/Piql_order_form.xlsx
+++ b/calc/static/calc/Piql_order_form.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="order" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'order'!$A$1:$H$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'order'!$A$1:$H$45</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
@@ -353,57 +353,74 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -412,38 +429,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -790,10 +790,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScale="96" zoomScaleNormal="55" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:H39"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="16.5"/>
@@ -807,165 +807,165 @@
     <col width="11.54296875" bestFit="1" customWidth="1" style="22" min="7" max="7"/>
     <col width="14" customWidth="1" style="22" min="8" max="8"/>
     <col width="11.26953125" bestFit="1" customWidth="1" style="22" min="9" max="9"/>
-    <col width="9.1796875" customWidth="1" style="22" min="10" max="47"/>
-    <col width="9.1796875" customWidth="1" style="22" min="48" max="16384"/>
+    <col width="9.1796875" customWidth="1" style="22" min="10" max="48"/>
+    <col width="9.1796875" customWidth="1" style="22" min="49" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
-      <c r="A1" s="26" t="n"/>
-      <c r="E1" s="21" t="inlineStr">
+      <c r="A1" s="23" t="n"/>
+      <c r="E1" s="55" t="inlineStr">
         <is>
           <t>Partner Order Form</t>
         </is>
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
-      <c r="A2" s="26" t="n"/>
+      <c r="A2" s="23" t="n"/>
     </row>
     <row r="3" ht="14.15" customHeight="1">
-      <c r="A3" s="41" t="n"/>
+      <c r="A3" s="48" t="n"/>
     </row>
     <row r="4" ht="14.15" customHeight="1">
-      <c r="A4" s="26" t="n"/>
-      <c r="E4" s="23" t="inlineStr">
+      <c r="A4" s="23" t="n"/>
+      <c r="E4" s="56" t="inlineStr">
         <is>
           <t>Date:</t>
         </is>
       </c>
-      <c r="G4" s="25" t="n">
-        <v>44090.44160509142</v>
+      <c r="G4" s="58" t="n">
+        <v>44100.42924320418</v>
       </c>
     </row>
     <row r="5" ht="14.15" customHeight="1">
-      <c r="A5" s="26" t="n"/>
-      <c r="E5" s="23" t="inlineStr">
+      <c r="A5" s="23" t="n"/>
+      <c r="E5" s="56" t="inlineStr">
         <is>
           <t>Piql Partner:</t>
         </is>
       </c>
-      <c r="G5" s="26" t="inlineStr">
+      <c r="G5" s="23" t="inlineStr">
         <is>
           <t>alfrtruj</t>
         </is>
       </c>
     </row>
     <row r="6" ht="14.15" customHeight="1">
-      <c r="A6" s="26" t="n"/>
-      <c r="E6" s="23" t="inlineStr">
+      <c r="A6" s="23" t="n"/>
+      <c r="E6" s="56" t="inlineStr">
         <is>
           <t>Partner Order Number:</t>
         </is>
       </c>
-      <c r="G6" s="27" t="n"/>
+      <c r="G6" s="59" t="n"/>
     </row>
     <row r="7" ht="14.15" customHeight="1">
-      <c r="A7" s="26" t="n"/>
-      <c r="E7" s="24" t="inlineStr">
+      <c r="A7" s="23" t="n"/>
+      <c r="E7" s="57" t="inlineStr">
         <is>
           <t>Customer name:</t>
         </is>
       </c>
-      <c r="G7" s="26" t="inlineStr">
-        <is>
-          <t>Kuben</t>
+      <c r="G7" s="23" t="inlineStr">
+        <is>
+          <t>Unesco</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="26" t="n"/>
+      <c r="A8" s="23" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="28" t="inlineStr">
+      <c r="A9" s="44" t="inlineStr">
         <is>
           <t>PIQL PARTNER &lt;Mandatory&gt;</t>
         </is>
       </c>
-      <c r="B9" s="29" t="n"/>
-      <c r="C9" s="29" t="n"/>
-      <c r="D9" s="29" t="n"/>
-      <c r="E9" s="30" t="n"/>
-      <c r="F9" s="28" t="inlineStr">
+      <c r="B9" s="25" t="n"/>
+      <c r="C9" s="25" t="n"/>
+      <c r="D9" s="25" t="n"/>
+      <c r="E9" s="34" t="n"/>
+      <c r="F9" s="44" t="inlineStr">
         <is>
           <t>Comments:</t>
         </is>
       </c>
-      <c r="G9" s="29" t="n"/>
-      <c r="H9" s="30" t="n"/>
+      <c r="G9" s="25" t="n"/>
+      <c r="H9" s="34" t="n"/>
     </row>
     <row r="10" ht="17.25" customHeight="1">
-      <c r="A10" s="46" t="inlineStr">
+      <c r="A10" s="53" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="B10" s="47" t="n"/>
-      <c r="C10" s="47" t="n"/>
-      <c r="D10" s="47" t="n"/>
-      <c r="E10" s="48" t="n"/>
-      <c r="F10" s="36" t="inlineStr">
-        <is>
-          <t>Comments about the job, logistics, shipment address (client contact details), special considerations, etc</t>
-        </is>
-      </c>
-      <c r="H10" s="34" t="n"/>
+      <c r="B10" s="41" t="n"/>
+      <c r="C10" s="41" t="n"/>
+      <c r="D10" s="41" t="n"/>
+      <c r="E10" s="42" t="n"/>
+      <c r="F10" s="45" t="inlineStr">
+        <is>
+          <t>Hoy</t>
+        </is>
+      </c>
+      <c r="H10" s="28" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="33" t="inlineStr">
+      <c r="A11" s="27" t="inlineStr">
         <is>
           <t>Contact person</t>
         </is>
       </c>
-      <c r="E11" s="34" t="n"/>
-      <c r="F11" s="37" t="n"/>
-      <c r="H11" s="34" t="n"/>
+      <c r="E11" s="28" t="n"/>
+      <c r="F11" s="46" t="n"/>
+      <c r="H11" s="28" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="57" t="inlineStr">
+      <c r="A12" s="29" t="inlineStr">
         <is>
           <t>Telephone</t>
         </is>
       </c>
-      <c r="E12" s="34" t="n"/>
-      <c r="F12" s="37" t="n"/>
-      <c r="H12" s="34" t="n"/>
+      <c r="E12" s="28" t="n"/>
+      <c r="F12" s="46" t="n"/>
+      <c r="H12" s="28" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="57" t="inlineStr">
+      <c r="A13" s="29" t="inlineStr">
         <is>
           <t>email:</t>
         </is>
       </c>
-      <c r="E13" s="34" t="n"/>
-      <c r="F13" s="37" t="n"/>
-      <c r="H13" s="34" t="n"/>
+      <c r="E13" s="28" t="n"/>
+      <c r="F13" s="46" t="n"/>
+      <c r="H13" s="28" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="33" t="n"/>
-      <c r="E14" s="34" t="n"/>
-      <c r="F14" s="37" t="n"/>
-      <c r="H14" s="34" t="n"/>
+      <c r="A14" s="27" t="n"/>
+      <c r="E14" s="28" t="n"/>
+      <c r="F14" s="46" t="n"/>
+      <c r="H14" s="28" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="58" t="n"/>
-      <c r="B15" s="39" t="n"/>
-      <c r="C15" s="39" t="n"/>
-      <c r="D15" s="39" t="n"/>
-      <c r="E15" s="40" t="n"/>
-      <c r="F15" s="38" t="n"/>
-      <c r="G15" s="39" t="n"/>
-      <c r="H15" s="40" t="n"/>
+      <c r="A15" s="30" t="n"/>
+      <c r="B15" s="31" t="n"/>
+      <c r="C15" s="31" t="n"/>
+      <c r="D15" s="31" t="n"/>
+      <c r="E15" s="32" t="n"/>
+      <c r="F15" s="47" t="n"/>
+      <c r="G15" s="31" t="n"/>
+      <c r="H15" s="32" t="n"/>
     </row>
     <row r="16" ht="30" customHeight="1">
-      <c r="A16" s="59" t="inlineStr">
+      <c r="A16" s="33" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="B16" s="29" t="n"/>
-      <c r="C16" s="29" t="n"/>
-      <c r="D16" s="29" t="n"/>
-      <c r="E16" s="30" t="n"/>
-      <c r="F16" s="59" t="inlineStr">
+      <c r="B16" s="25" t="n"/>
+      <c r="C16" s="25" t="n"/>
+      <c r="D16" s="25" t="n"/>
+      <c r="E16" s="34" t="n"/>
+      <c r="F16" s="33" t="inlineStr">
         <is>
           <t>Qty</t>
         </is>
@@ -987,76 +987,66 @@
           <t>1. Offline Storage (one-off payment)</t>
         </is>
       </c>
-      <c r="B17" s="29" t="n"/>
-      <c r="C17" s="29" t="n"/>
-      <c r="D17" s="29" t="n"/>
-      <c r="E17" s="30" t="n"/>
+      <c r="B17" s="25" t="n"/>
+      <c r="C17" s="25" t="n"/>
+      <c r="D17" s="25" t="n"/>
+      <c r="E17" s="34" t="n"/>
       <c r="F17" s="2" t="n"/>
       <c r="G17" s="9" t="n"/>
       <c r="H17" s="10" t="n"/>
     </row>
     <row r="18" ht="16.5" customHeight="1">
-      <c r="A18" s="32" t="inlineStr">
+      <c r="A18" s="36" t="inlineStr">
         <is>
           <t>piqlConnect (only piqlFilm)</t>
         </is>
       </c>
-      <c r="B18" s="29" t="n"/>
-      <c r="C18" s="29" t="n"/>
-      <c r="D18" s="29" t="n"/>
-      <c r="E18" s="30" t="n"/>
+      <c r="B18" s="25" t="n"/>
+      <c r="C18" s="25" t="n"/>
+      <c r="D18" s="25" t="n"/>
+      <c r="E18" s="34" t="n"/>
       <c r="F18" s="2" t="n"/>
       <c r="G18" s="9" t="n"/>
       <c r="H18" s="10" t="n"/>
     </row>
     <row r="19" ht="17.25" customHeight="1">
-      <c r="A19" s="32" t="inlineStr">
+      <c r="A19" s="36" t="inlineStr">
         <is>
           <t>Digital (GB)</t>
         </is>
       </c>
-      <c r="B19" s="29" t="n"/>
-      <c r="C19" s="29" t="n"/>
-      <c r="D19" s="29" t="n"/>
-      <c r="E19" s="30" t="n"/>
+      <c r="B19" s="25" t="n"/>
+      <c r="C19" s="25" t="n"/>
+      <c r="D19" s="25" t="n"/>
+      <c r="E19" s="34" t="n"/>
       <c r="F19" s="14" t="n">
-        <v>360</v>
+        <v>240</v>
       </c>
       <c r="G19" s="9" t="n">
         <v>15</v>
       </c>
       <c r="H19" s="10" t="n">
-        <v>3600</v>
+        <v>1800</v>
       </c>
       <c r="I19" s="16" t="n"/>
     </row>
     <row r="20" ht="17.25" customHeight="1">
-      <c r="A20" s="31" t="inlineStr">
+      <c r="A20" s="37" t="inlineStr">
         <is>
           <t>Visual (pages)</t>
         </is>
       </c>
-      <c r="B20" s="29" t="n"/>
-      <c r="C20" s="29" t="n"/>
+      <c r="B20" s="25" t="n"/>
+      <c r="C20" s="25" t="n"/>
       <c r="D20" s="7" t="inlineStr">
         <is>
           <t>Pages/frame:</t>
         </is>
       </c>
-      <c r="E20" s="8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F20" s="15" t="n">
-        <v>130000</v>
-      </c>
-      <c r="G20" s="11" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="H20" s="10" t="n">
-        <v>3900</v>
-      </c>
+      <c r="E20" s="8" t="n"/>
+      <c r="F20" s="15" t="n"/>
+      <c r="G20" s="11" t="n"/>
+      <c r="H20" s="10" t="n"/>
       <c r="I20" s="16" t="n"/>
     </row>
     <row r="21" ht="17.25" customHeight="1">
@@ -1065,10 +1055,10 @@
           <t>2. Online Storage (GB) - piqlConnect (1 TB &amp; 1 piqlFilm included)</t>
         </is>
       </c>
-      <c r="B21" s="29" t="n"/>
-      <c r="C21" s="29" t="n"/>
-      <c r="D21" s="29" t="n"/>
-      <c r="E21" s="30" t="n"/>
+      <c r="B21" s="25" t="n"/>
+      <c r="C21" s="25" t="n"/>
+      <c r="D21" s="25" t="n"/>
+      <c r="E21" s="34" t="n"/>
       <c r="F21" s="2" t="n">
         <v>1</v>
       </c>
@@ -1081,13 +1071,13 @@
       <c r="I21" s="16" t="n"/>
     </row>
     <row r="22" ht="17.25" customHeight="1">
-      <c r="A22" s="31" t="inlineStr">
+      <c r="A22" s="37" t="inlineStr">
         <is>
           <t xml:space="preserve">Online Storage (GB) </t>
         </is>
       </c>
-      <c r="B22" s="29" t="n"/>
-      <c r="C22" s="29" t="n"/>
+      <c r="B22" s="25" t="n"/>
+      <c r="C22" s="25" t="n"/>
       <c r="D22" s="3" t="inlineStr">
         <is>
           <t>Payment:</t>
@@ -1099,13 +1089,13 @@
         </is>
       </c>
       <c r="F22" s="2" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="G22" s="11" t="n">
         <v>0.576</v>
       </c>
       <c r="H22" s="10" t="n">
-        <v>576</v>
+        <v>1152</v>
       </c>
       <c r="I22" s="16" t="n"/>
     </row>
@@ -1115,25 +1105,25 @@
           <t xml:space="preserve">3. Arctic World Archive </t>
         </is>
       </c>
-      <c r="B23" s="29" t="n"/>
-      <c r="C23" s="29" t="n"/>
-      <c r="D23" s="29" t="n"/>
-      <c r="E23" s="30" t="n"/>
+      <c r="B23" s="25" t="n"/>
+      <c r="C23" s="25" t="n"/>
+      <c r="D23" s="25" t="n"/>
+      <c r="E23" s="34" t="n"/>
       <c r="F23" s="2" t="n"/>
       <c r="G23" s="9" t="n"/>
       <c r="H23" s="10" t="n"/>
       <c r="I23" s="16" t="n"/>
     </row>
     <row r="24" ht="16.5" customHeight="1">
-      <c r="A24" s="32" t="inlineStr">
+      <c r="A24" s="36" t="inlineStr">
         <is>
           <t>Registration fee</t>
         </is>
       </c>
-      <c r="B24" s="29" t="n"/>
-      <c r="C24" s="29" t="n"/>
-      <c r="D24" s="29" t="n"/>
-      <c r="E24" s="30" t="n"/>
+      <c r="B24" s="25" t="n"/>
+      <c r="C24" s="25" t="n"/>
+      <c r="D24" s="25" t="n"/>
+      <c r="E24" s="34" t="n"/>
       <c r="F24" s="2" t="n">
         <v>1</v>
       </c>
@@ -1146,13 +1136,13 @@
       <c r="I24" s="16" t="n"/>
     </row>
     <row r="25" ht="16.5" customHeight="1">
-      <c r="A25" s="31" t="inlineStr">
+      <c r="A25" s="37" t="inlineStr">
         <is>
           <t xml:space="preserve">AWA contribution </t>
         </is>
       </c>
-      <c r="B25" s="29" t="n"/>
-      <c r="C25" s="29" t="n"/>
+      <c r="B25" s="25" t="n"/>
+      <c r="C25" s="25" t="n"/>
       <c r="D25" s="3" t="inlineStr">
         <is>
           <t>Entity:</t>
@@ -1175,15 +1165,15 @@
       <c r="I25" s="16" t="n"/>
     </row>
     <row r="26" ht="16.5" customHeight="1">
-      <c r="A26" s="32" t="inlineStr">
+      <c r="A26" s="36" t="inlineStr">
         <is>
           <t>Management fee (per period)</t>
         </is>
       </c>
-      <c r="B26" s="29" t="n"/>
-      <c r="C26" s="29" t="n"/>
-      <c r="D26" s="29" t="n"/>
-      <c r="E26" s="30" t="n"/>
+      <c r="B26" s="25" t="n"/>
+      <c r="C26" s="25" t="n"/>
+      <c r="D26" s="25" t="n"/>
+      <c r="E26" s="34" t="n"/>
       <c r="F26" s="2" t="inlineStr">
         <is>
           <t>5</t>
@@ -1198,13 +1188,13 @@
       <c r="I26" s="16" t="n"/>
     </row>
     <row r="27" ht="17.5" customHeight="1">
-      <c r="A27" s="31" t="inlineStr">
+      <c r="A27" s="37" t="inlineStr">
         <is>
           <t>Storage (per reel / per period)</t>
         </is>
       </c>
-      <c r="B27" s="29" t="n"/>
-      <c r="C27" s="29" t="n"/>
+      <c r="B27" s="25" t="n"/>
+      <c r="C27" s="25" t="n"/>
       <c r="D27" s="3" t="inlineStr">
         <is>
           <t>Period (years):</t>
@@ -1216,13 +1206,13 @@
         </is>
       </c>
       <c r="F27" s="2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G27" s="9" t="n">
         <v>60</v>
       </c>
       <c r="H27" s="10" t="n">
-        <v>1500</v>
+        <v>600</v>
       </c>
       <c r="I27" s="16" t="n"/>
     </row>
@@ -1232,10 +1222,10 @@
           <t>4. Professional Services (per day)</t>
         </is>
       </c>
-      <c r="B28" s="29" t="n"/>
-      <c r="C28" s="29" t="n"/>
-      <c r="D28" s="29" t="n"/>
-      <c r="E28" s="30" t="n"/>
+      <c r="B28" s="25" t="n"/>
+      <c r="C28" s="25" t="n"/>
+      <c r="D28" s="25" t="n"/>
+      <c r="E28" s="34" t="n"/>
       <c r="F28" s="2" t="n">
         <v>1</v>
       </c>
@@ -1253,10 +1243,10 @@
           <t xml:space="preserve">5. piqlReader </t>
         </is>
       </c>
-      <c r="B29" s="29" t="n"/>
-      <c r="C29" s="29" t="n"/>
-      <c r="D29" s="29" t="n"/>
-      <c r="E29" s="30" t="n"/>
+      <c r="B29" s="25" t="n"/>
+      <c r="C29" s="25" t="n"/>
+      <c r="D29" s="25" t="n"/>
+      <c r="E29" s="34" t="n"/>
       <c r="F29" s="2" t="n">
         <v>1</v>
       </c>
@@ -1269,15 +1259,15 @@
       <c r="I29" s="16" t="n"/>
     </row>
     <row r="30" ht="17.25" customHeight="1">
-      <c r="A30" s="32" t="inlineStr">
+      <c r="A30" s="36" t="inlineStr">
         <is>
           <t>Installation and training</t>
         </is>
       </c>
-      <c r="B30" s="29" t="n"/>
-      <c r="C30" s="29" t="n"/>
-      <c r="D30" s="29" t="n"/>
-      <c r="E30" s="30" t="n"/>
+      <c r="B30" s="25" t="n"/>
+      <c r="C30" s="25" t="n"/>
+      <c r="D30" s="25" t="n"/>
+      <c r="E30" s="34" t="n"/>
       <c r="F30" s="2" t="n">
         <v>1</v>
       </c>
@@ -1290,13 +1280,13 @@
       <c r="I30" s="16" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="56" t="inlineStr">
+      <c r="A31" s="26" t="inlineStr">
         <is>
           <t>Service agreement (per year)</t>
         </is>
       </c>
-      <c r="B31" s="29" t="n"/>
-      <c r="C31" s="29" t="n"/>
+      <c r="B31" s="25" t="n"/>
+      <c r="C31" s="25" t="n"/>
       <c r="D31" s="5" t="inlineStr">
         <is>
           <t>Type:</t>
@@ -1319,141 +1309,181 @@
       <c r="I31" s="16" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="55" t="inlineStr">
+      <c r="A32" s="24" t="inlineStr">
         <is>
           <t>6. Shipment cost</t>
         </is>
       </c>
-      <c r="B32" s="29" t="n"/>
-      <c r="C32" s="29" t="n"/>
+      <c r="B32" s="25" t="n"/>
+      <c r="C32" s="25" t="n"/>
       <c r="D32" s="5" t="inlineStr">
         <is>
           <t>Reels</t>
         </is>
       </c>
       <c r="E32" s="6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F32" s="2" t="n"/>
       <c r="G32" s="9" t="n">
         <v>20</v>
       </c>
       <c r="H32" s="10" t="n">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="I32" s="16" t="n"/>
     </row>
     <row r="33" ht="16.5" customHeight="1">
-      <c r="A33" s="50" t="n"/>
-      <c r="G33" s="52" t="inlineStr">
+      <c r="A33" s="38" t="n"/>
+      <c r="G33" s="40" t="inlineStr">
         <is>
           <t xml:space="preserve">TOTAL </t>
         </is>
       </c>
       <c r="H33" s="12" t="n">
-        <v>105856</v>
+        <v>99772</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="53" t="n"/>
-      <c r="D34" s="34" t="n"/>
-      <c r="E34" s="52" t="inlineStr">
+      <c r="A34" s="43" t="n"/>
+      <c r="D34" s="28" t="n"/>
+      <c r="E34" s="40" t="inlineStr">
         <is>
           <t>Total to pay from the second term</t>
         </is>
       </c>
-      <c r="F34" s="47" t="n"/>
-      <c r="G34" s="48" t="n"/>
+      <c r="F34" s="41" t="n"/>
+      <c r="G34" s="42" t="n"/>
       <c r="H34" s="13" t="n">
-        <v>11956</v>
+        <v>12532</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="26" t="n"/>
+      <c r="A35" s="51" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="51" t="inlineStr">
+      <c r="A36" s="39" t="inlineStr">
         <is>
           <t>Delivery terms: three weeks after the data is received by Piql. ExWorks, Drammen.</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="54" t="inlineStr">
+      <c r="A37" s="21" t="inlineStr">
         <is>
           <t xml:space="preserve">Payment terms 100% on delivery </t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="51" t="inlineStr">
+      <c r="A38" s="39" t="inlineStr">
         <is>
           <t xml:space="preserve">Notes: To provide technical and account information to the production department. Fill out this form: </t>
         </is>
       </c>
-      <c r="B38" s="51" t="n"/>
-      <c r="C38" s="51" t="n"/>
-      <c r="D38" s="51" t="n"/>
-      <c r="E38" s="51" t="n"/>
-      <c r="F38" s="51" t="n"/>
-      <c r="G38" s="51" t="n"/>
-      <c r="H38" s="51" t="n"/>
+      <c r="B38" s="39" t="n"/>
+      <c r="C38" s="39" t="n"/>
+      <c r="D38" s="39" t="n"/>
+      <c r="E38" s="39" t="n"/>
+      <c r="F38" s="39" t="n"/>
+      <c r="G38" s="39" t="n"/>
+      <c r="H38" s="39" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="49" t="inlineStr">
+      <c r="A39" s="54" t="inlineStr">
         <is>
           <t>piqlFilm production form - use this online form to specify the parameters to produce piqlFilm</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="44" t="n"/>
+      <c r="A40" s="51" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="41" t="inlineStr">
+      <c r="A41" s="48" t="inlineStr">
         <is>
           <t>Send this order to orders@piql.com. If you have any questions concerning this ORDER please contact:</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="45" t="inlineStr">
+      <c r="A42" s="52" t="inlineStr">
         <is>
           <t>Espen Berge Kvam</t>
         </is>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="49" t="inlineStr">
+      <c r="A43" s="54" t="inlineStr">
         <is>
           <t>espen.berge.kvam@piql.com</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="42" t="inlineStr">
+      <c r="A44" s="49" t="inlineStr">
         <is>
           <t>+47 94030050</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="41" t="n"/>
+      <c r="A45" s="48" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="41" t="n"/>
+      <c r="A46" s="22" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="22" t="n"/>
+      <c r="A47" s="50" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="43" t="n"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="22" t="n"/>
+      <c r="A48" s="22" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="59">
+    <mergeCell ref="E1:H2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H15"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A47:H47"/>
+    <mergeCell ref="A46:H46"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A42:H42"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A43:H43"/>
+    <mergeCell ref="A45:H45"/>
+    <mergeCell ref="A39:H39"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="A34:D34"/>
     <mergeCell ref="A37:H37"/>
     <mergeCell ref="A35:H35"/>
     <mergeCell ref="A32:C32"/>
@@ -1470,53 +1500,9 @@
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H15"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A49:H49"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="A47:H47"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="A42:H42"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A43:H43"/>
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="A46:H46"/>
-    <mergeCell ref="A39:H39"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E1:H2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A39" display="piqlFilm production form - use this online form to specify the parameters to produce piqlFilm" r:id="rId1"/>
+    <hyperlink ref="A39" r:id="rId1"/>
     <hyperlink ref="A43" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.46875" top="0.4791666666666667" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add download order form
</commit_message>
<xml_diff>
--- a/calc/static/calc/Piql_order_form.xlsx
+++ b/calc/static/calc/Piql_order_form.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlfredoTrujillo\PycharmProjects\calculator\calc\static\calc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlfredoTrujillo\Documents\Piql (no sync)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02A5591-A545-44CE-B4B3-BC831DD647D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B18BE4C6-AF35-4CD4-BEA4-6E225363BCE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33675" yWindow="2550" windowWidth="14400" windowHeight="7455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="29020" windowHeight="17770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="order" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">order!$A$1:$H$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">order!$A$1:$H$45</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Partner Order Form</t>
   </si>
@@ -43,7 +43,7 @@
     <t>Customer name:</t>
   </si>
   <si>
-    <t>Trujillo AS</t>
+    <t>Ikea</t>
   </si>
   <si>
     <t>PIQL PARTNER &lt;Mandatory&gt;</t>
@@ -55,7 +55,7 @@
     <t>Address</t>
   </si>
   <si>
-    <t>El texto</t>
+    <t>hoyo</t>
   </si>
   <si>
     <t>Contact person</t>
@@ -97,7 +97,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>2. Online Storage (GB) - piqlConnect (1 TB &amp; 1 piqlFilm included)</t>
+    <t>2. Online Storage (GB) - piqlConnect (1 Terabyte &amp; 1 piqlFilm included)</t>
   </si>
   <si>
     <t xml:space="preserve">Online Storage (GB) </t>
@@ -121,9 +121,15 @@
     <t>Entity:</t>
   </si>
   <si>
+    <t>public</t>
+  </si>
+  <si>
     <t>Management fee (per period)</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>Storage (per reel / per period)</t>
   </si>
   <si>
@@ -169,6 +175,9 @@
     <t xml:space="preserve">Notes: To provide technical and account information to the production department. Fill out this form: </t>
   </si>
   <si>
+    <t>piqlFilm production form - use this online form to specify the parameters to produce piqlFilm</t>
+  </si>
+  <si>
     <t>Send this order to orders@piql.com. If you have any questions concerning this ORDER please contact:</t>
   </si>
   <si>
@@ -179,9 +188,6 @@
   </si>
   <si>
     <t>+47 94030050</t>
-  </si>
-  <si>
-    <t>piqlFilm Production form - use this online form for specifying the parameters for the film production</t>
   </si>
 </sst>
 </file>
@@ -475,7 +481,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -524,97 +530,100 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -898,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="96" zoomScaleNormal="55" zoomScalePageLayoutView="96" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:H40"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="16.5" x14ac:dyDescent="0.5"/>
@@ -915,16 +924,16 @@
     <col min="7" max="7" width="11.54296875" style="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="17" customWidth="1"/>
     <col min="9" max="9" width="11.26953125" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="47" width="9.1796875" style="17" customWidth="1"/>
-    <col min="48" max="16384" width="9.1796875" style="17"/>
+    <col min="10" max="50" width="9.1796875" style="17" customWidth="1"/>
+    <col min="51" max="16384" width="9.1796875" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="26"/>
+      <c r="A1" s="52"/>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="56" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="22"/>
@@ -932,7 +941,7 @@
       <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="26"/>
+      <c r="A2" s="52"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -942,7 +951,7 @@
       <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="41"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
@@ -952,61 +961,61 @@
       <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="26"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="57" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="22"/>
-      <c r="G4" s="25">
-        <v>44080.874444652407</v>
+      <c r="G4" s="59">
+        <v>44100.496798426568</v>
       </c>
       <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="26"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="22"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="57" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="22"/>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="52" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="26"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="57" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="22"/>
-      <c r="G6" s="27"/>
+      <c r="G6" s="60"/>
       <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8" ht="14.15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="26"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="58" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="22"/>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="52" t="s">
         <v>6</v>
       </c>
       <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A8" s="26"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -1016,98 +1025,98 @@
       <c r="H8" s="22"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="28" t="s">
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="29"/>
-      <c r="H9" s="30"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="34"/>
     </row>
     <row r="10" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="36" t="s">
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="44" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="22"/>
-      <c r="H10" s="34"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="27" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="37"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="45"/>
       <c r="G11" s="22"/>
-      <c r="H11" s="34"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="29" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="37"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="45"/>
       <c r="G12" s="22"/>
-      <c r="H12" s="34"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="29" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="37"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="45"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="34"/>
+      <c r="H13" s="28"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A14" s="33"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="37"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="45"/>
       <c r="G14" s="22"/>
-      <c r="H14" s="34"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A15" s="58"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="40"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="32"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="18" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="20" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1121,45 +1130,51 @@
       <c r="A17" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="30"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="34"/>
       <c r="F17" s="2"/>
       <c r="G17" s="9"/>
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="30"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="34"/>
       <c r="F18" s="2"/>
       <c r="G18" s="9"/>
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="10"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="14">
+        <v>240</v>
+      </c>
+      <c r="G19" s="9">
+        <v>15</v>
+      </c>
+      <c r="H19" s="10">
+        <v>1800</v>
+      </c>
       <c r="I19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="7" t="s">
         <v>22</v>
       </c>
@@ -1167,24 +1182,24 @@
         <v>23</v>
       </c>
       <c r="F20" s="15">
-        <v>89000</v>
+        <v>65000</v>
       </c>
       <c r="G20" s="11">
         <v>0.03</v>
       </c>
       <c r="H20" s="10">
-        <v>720</v>
+        <v>1950</v>
       </c>
       <c r="I20" s="16"/>
     </row>
     <row r="21" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="30"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="34"/>
       <c r="F21" s="2">
         <v>1</v>
       </c>
@@ -1197,11 +1212,11 @@
       <c r="I21" s="16"/>
     </row>
     <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
       <c r="D22" s="3" t="s">
         <v>26</v>
       </c>
@@ -1209,13 +1224,13 @@
         <v>27</v>
       </c>
       <c r="F22" s="2">
-        <v>6000</v>
+        <v>10000</v>
       </c>
       <c r="G22" s="11">
-        <v>0.57599999999999996</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="H22" s="10">
-        <v>2880</v>
+        <v>432</v>
       </c>
       <c r="I22" s="16"/>
     </row>
@@ -1223,92 +1238,126 @@
       <c r="A23" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="30"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="34"/>
       <c r="F23" s="2"/>
       <c r="G23" s="9"/>
       <c r="H23" s="10"/>
       <c r="I23" s="16"/>
     </row>
     <row r="24" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="10"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+      <c r="G24" s="9">
+        <v>200</v>
+      </c>
+      <c r="H24" s="10">
+        <v>200</v>
+      </c>
       <c r="I24" s="16"/>
     </row>
     <row r="25" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
       <c r="D25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="10"/>
+      <c r="E25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="9">
+        <v>500</v>
+      </c>
+      <c r="H25" s="10">
+        <v>500</v>
+      </c>
       <c r="I25" s="16"/>
     </row>
     <row r="26" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="10"/>
+      <c r="A26" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="9">
+        <v>60</v>
+      </c>
+      <c r="H26" s="10">
+        <v>300</v>
+      </c>
       <c r="I26" s="16"/>
     </row>
     <row r="27" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
+      <c r="A27" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
       <c r="D27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="10"/>
+      <c r="F27" s="2">
+        <v>3</v>
+      </c>
+      <c r="G27" s="9">
+        <v>60</v>
+      </c>
+      <c r="H27" s="10">
+        <v>900</v>
+      </c>
       <c r="I27" s="16"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A28" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="10"/>
+        <v>37</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="9">
+        <v>900</v>
+      </c>
+      <c r="H28" s="10">
+        <v>900</v>
+      </c>
       <c r="I28" s="16"/>
     </row>
     <row r="29" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A29" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="30"/>
+        <v>38</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="34"/>
       <c r="F29" s="2">
         <v>1</v>
       </c>
@@ -1321,13 +1370,13 @@
       <c r="I29" s="16"/>
     </row>
     <row r="30" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
+      <c r="A30" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="34"/>
       <c r="F30" s="2">
         <v>1</v>
       </c>
@@ -1340,16 +1389,16 @@
       <c r="I30" s="16"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A31" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
+      <c r="A31" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
       <c r="D31" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F31" s="2">
         <v>1</v>
@@ -1363,20 +1412,20 @@
       <c r="I31" s="16"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A32" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
+      <c r="A32" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
       <c r="D32" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E32" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="9">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H32" s="10">
         <v>60</v>
@@ -1384,35 +1433,35 @@
       <c r="I32" s="16"/>
     </row>
     <row r="33" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="50"/>
+      <c r="A33" s="54"/>
       <c r="B33" s="22"/>
       <c r="C33" s="22"/>
       <c r="D33" s="22"/>
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
-      <c r="G33" s="20" t="s">
-        <v>43</v>
+      <c r="G33" s="19" t="s">
+        <v>45</v>
       </c>
       <c r="H33" s="12">
-        <v>97880</v>
+        <v>101322</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A34" s="53"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="47"/>
-      <c r="G34" s="48"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="40"/>
+      <c r="G34" s="41"/>
       <c r="H34" s="13">
-        <v>14260</v>
+        <v>11812</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A35" s="26"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
@@ -1422,8 +1471,8 @@
       <c r="H35" s="22"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A36" s="51" t="s">
-        <v>45</v>
+      <c r="A36" s="38" t="s">
+        <v>47</v>
       </c>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
@@ -1434,8 +1483,8 @@
       <c r="H36" s="22"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A37" s="54" t="s">
-        <v>46</v>
+      <c r="A37" s="21" t="s">
+        <v>48</v>
       </c>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
@@ -1446,31 +1495,31 @@
       <c r="H37" s="22"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A38" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
+      <c r="A38" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A39" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" s="49"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49"/>
+      <c r="A39" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A40" s="44"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="D40" s="22"/>
@@ -1480,8 +1529,8 @@
       <c r="H40" s="22"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A41" s="41" t="s">
-        <v>48</v>
+      <c r="A41" s="47" t="s">
+        <v>51</v>
       </c>
       <c r="B41" s="22"/>
       <c r="C41" s="22"/>
@@ -1492,8 +1541,8 @@
       <c r="H41" s="22"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A42" s="45" t="s">
-        <v>49</v>
+      <c r="A42" s="50" t="s">
+        <v>52</v>
       </c>
       <c r="B42" s="22"/>
       <c r="C42" s="22"/>
@@ -1504,8 +1553,8 @@
       <c r="H42" s="22"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A43" s="49" t="s">
-        <v>50</v>
+      <c r="A43" s="53" t="s">
+        <v>53</v>
       </c>
       <c r="B43" s="22"/>
       <c r="C43" s="22"/>
@@ -1516,8 +1565,8 @@
       <c r="H43" s="22"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A44" s="42" t="s">
-        <v>51</v>
+      <c r="A44" s="48" t="s">
+        <v>54</v>
       </c>
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
@@ -1528,7 +1577,7 @@
       <c r="H44" s="22"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A45" s="41"/>
+      <c r="A45" s="47"/>
       <c r="B45" s="22"/>
       <c r="C45" s="22"/>
       <c r="D45" s="22"/>
@@ -1538,7 +1587,7 @@
       <c r="H45" s="22"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A46" s="41"/>
+      <c r="A46" s="22"/>
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
       <c r="D46" s="22"/>
@@ -1548,7 +1597,7 @@
       <c r="H46" s="22"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A47" s="22"/>
+      <c r="A47" s="49"/>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
       <c r="D47" s="22"/>
@@ -1558,7 +1607,7 @@
       <c r="H47" s="22"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A48" s="43"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
       <c r="D48" s="22"/>
@@ -1567,18 +1616,51 @@
       <c r="G48" s="22"/>
       <c r="H48" s="22"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A49" s="22"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
-    </row>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="59">
+    <mergeCell ref="E1:H2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H15"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A48:H48"/>
+    <mergeCell ref="A44:H44"/>
+    <mergeCell ref="A47:H47"/>
+    <mergeCell ref="A46:H46"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A42:H42"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A43:H43"/>
+    <mergeCell ref="A45:H45"/>
+    <mergeCell ref="A39:H39"/>
+    <mergeCell ref="A33:F33"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="A34:D34"/>
     <mergeCell ref="A37:H37"/>
     <mergeCell ref="A35:H35"/>
     <mergeCell ref="A32:C32"/>
@@ -1595,58 +1677,13 @@
     <mergeCell ref="A19:E19"/>
     <mergeCell ref="A20:C20"/>
     <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A33:F33"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H15"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A49:H49"/>
-    <mergeCell ref="A44:H44"/>
-    <mergeCell ref="A48:H48"/>
-    <mergeCell ref="A47:H47"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="A42:H42"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A43:H43"/>
-    <mergeCell ref="A45:H45"/>
-    <mergeCell ref="A46:H46"/>
-    <mergeCell ref="A39:H39"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E1:H2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A39" r:id="rId1" display="https://forms.office.com/Pages/ResponsePage.aspx?id=k4yqUSxZRkSwWH0R7QU1A3pm4lZOZiVDhXIaxSEWbBVUM1NPUEw3OTcwMTNLQTcwVzNNOVFST1NEOC4u" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A39" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="A43" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A39:H39" r:id="rId3" display="piqlFilm Production form - use this online form for specifying the parameters for the film production" xr:uid="{4D2A558B-6153-4B4B-9642-4094CD2FBA41}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.46875" top="0.47916666666666669" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;K05+000Piql AS&amp;K08+000 | &amp;K05+000Grønland 56, 3045 Drammen&amp;K08+000 |&amp;K05+000 NORWAY&amp;K08+000 | &amp;K05+000Ph: +47 905 33 432&amp;K08+000</oddFooter>
   </headerFooter>

</xml_diff>